<commit_message>
add : CGA75-P001 CAM
</commit_message>
<xml_diff>
--- a/機械設計/_BOM/BOM.xlsx
+++ b/機械設計/_BOM/BOM.xlsx
@@ -8,11 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\GitHub\2022-KawasakiRobot\機械設計\_BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE298BB-EBAD-49E5-8B78-BF36E7AD68C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449B149F-FEF2-42DB-88EB-0FC5E14F5BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="13410" windowWidth="29040" windowHeight="15840" xr2:uid="{32AE311B-7C41-46B2-8E02-C1E406B74BE1}"/>
-    <workbookView xWindow="38280" yWindow="6090" windowWidth="19440" windowHeight="15000" xr2:uid="{00A973FC-FE82-4E58-861A-5408EBDAA23E}"/>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{F6B6BD99-36AE-468F-8B2F-9AA042AEB062}"/>
+    <workbookView xWindow="-28920" yWindow="13410" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{F6B6BD99-36AE-468F-8B2F-9AA042AEB062}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2205" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2207" uniqueCount="341">
   <si>
     <t>種類</t>
   </si>
@@ -1164,6 +1162,20 @@
     <rPh sb="0" eb="2">
       <t>シュザイ</t>
     </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>材料型式</t>
+    <rPh sb="0" eb="2">
+      <t>ザイリョウ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>カタシキ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>A2017-BP-80-25</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1635,11 +1647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B61C4854-7AE2-455B-B515-BBA850988212}">
   <dimension ref="A1:T241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B73" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L127" sqref="L127"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
@@ -13794,10 +13802,6 @@
   <dimension ref="A1:C143"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView topLeftCell="A73" zoomScale="115" zoomScaleNormal="115" workbookViewId="1">
-      <selection activeCell="E1" sqref="E1:H1048576"/>
-    </sheetView>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -15671,9 +15675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1F7574-C968-489E-91DC-0C793DF8D9FA}">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2">
+    <sheetView workbookViewId="0">
       <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
@@ -16594,23 +16596,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A131F5D-359C-447A-A38B-BF4A40019FE6}">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="2">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="28.125" customWidth="1"/>
+    <col min="1" max="1" width="21.625" customWidth="1"/>
     <col min="2" max="2" width="27.375" customWidth="1"/>
-    <col min="3" max="3" width="15.125" customWidth="1"/>
-    <col min="4" max="7" width="8.75" customWidth="1"/>
+    <col min="3" max="3" width="12.875" customWidth="1"/>
+    <col min="4" max="4" width="15.125" customWidth="1"/>
+    <col min="5" max="8" width="8.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.4">
       <c r="A1" s="13" t="s">
         <v>332</v>
       </c>
@@ -16621,19 +16622,22 @@
         <v>334</v>
       </c>
       <c r="D1" s="13" t="s">
+        <v>339</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>338</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>335</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>336</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" t="str" cm="1">
         <f t="array" ref="A2:A59">_xlfn._xlws.SORT(_xlfn._xlws.FILTER(Sheet2!B22:B79,Sheet2!B22:B79&lt;&gt;""))</f>
         <v>CGA75-P001</v>
@@ -16646,9 +16650,13 @@
         <f>_xlfn.XLOOKUP(A2,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D2" s="9"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="D2" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" t="str">
         <v>CGA75-P002</v>
       </c>
@@ -16661,8 +16669,9 @@
         <v>A2017</v>
       </c>
       <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" t="str">
         <v>CGA75-P003</v>
       </c>
@@ -16675,8 +16684,9 @@
         <v>A2017</v>
       </c>
       <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" t="str">
         <v>CGA75-P004</v>
       </c>
@@ -16689,8 +16699,9 @@
         <v>S45C</v>
       </c>
       <c r="D5" s="9"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" t="str">
         <v>CGA75-RS380-4-P001</v>
       </c>
@@ -16703,8 +16714,9 @@
         <v>A2017</v>
       </c>
       <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" t="str">
         <v>CGA75-RS380-4-P002</v>
       </c>
@@ -16717,8 +16729,9 @@
         <v>A2017</v>
       </c>
       <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" t="str">
         <v>CU-AAS001-P001</v>
       </c>
@@ -16731,8 +16744,9 @@
         <v>A2017</v>
       </c>
       <c r="D8" s="9"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" t="str">
         <v>CU-AAS002-P001</v>
       </c>
@@ -16745,8 +16759,9 @@
         <v>A2017</v>
       </c>
       <c r="D9" s="9"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" t="str">
         <v>CU-AAS002-P002</v>
       </c>
@@ -16759,8 +16774,9 @@
         <v>A2017</v>
       </c>
       <c r="D10" s="9"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" t="str">
         <v>CU-AAS002-P003</v>
       </c>
@@ -16773,8 +16789,9 @@
         <v>A2017</v>
       </c>
       <c r="D11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12" t="str">
         <v>CU-AAS003L-P001</v>
       </c>
@@ -16787,8 +16804,9 @@
         <v>A2017</v>
       </c>
       <c r="D12" s="9"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13" t="str">
         <v>CU-AAS003-P001</v>
       </c>
@@ -16801,8 +16819,9 @@
         <v>A2017</v>
       </c>
       <c r="D13" s="9"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14" t="str">
         <v>CU-AAS003R-P001</v>
       </c>
@@ -16815,8 +16834,9 @@
         <v>A2017</v>
       </c>
       <c r="D14" s="9"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E14" s="9"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15" t="str">
         <v>CU-AAS-P001</v>
       </c>
@@ -16829,8 +16849,9 @@
         <v>A2017</v>
       </c>
       <c r="D15" s="9"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E15" s="9"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16" t="str">
         <v>CU-AAS-P002</v>
       </c>
@@ -16843,8 +16864,9 @@
         <v>A2017</v>
       </c>
       <c r="D16" s="9"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" t="str">
         <v>CU-AAS-P003</v>
       </c>
@@ -16857,8 +16879,9 @@
         <v>AR-M2</v>
       </c>
       <c r="D17" s="9"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" t="str">
         <v>CU-AAS-P004</v>
       </c>
@@ -16871,8 +16894,9 @@
         <v>AR-M2</v>
       </c>
       <c r="D18" s="9"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E18" s="9"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" t="str">
         <v>CU-P001</v>
       </c>
@@ -16885,8 +16909,9 @@
         <v>AR-M2</v>
       </c>
       <c r="D19" s="9"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" t="str">
         <v>CU-P002</v>
       </c>
@@ -16899,8 +16924,9 @@
         <v>A2017</v>
       </c>
       <c r="D20" s="9"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E20" s="9"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21" t="str">
         <v>CU-SAS001-P001</v>
       </c>
@@ -16913,8 +16939,9 @@
         <v>A2017</v>
       </c>
       <c r="D21" s="9"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E21" s="9"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" t="str">
         <v>CU-SAS001-P002</v>
       </c>
@@ -16927,8 +16954,9 @@
         <v>A2017</v>
       </c>
       <c r="D22" s="9"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E22" s="9"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" t="str">
         <v>CU-SAS001-P003</v>
       </c>
@@ -16941,8 +16969,9 @@
         <v>A2017</v>
       </c>
       <c r="D23" s="9"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E23" s="9"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" t="str">
         <v>CU-SAS002-P001</v>
       </c>
@@ -16955,8 +16984,9 @@
         <v>A2017</v>
       </c>
       <c r="D24" s="9"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E24" s="9"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25" t="str">
         <v>CU-SAS002-P002</v>
       </c>
@@ -16969,8 +16999,9 @@
         <v>A2017</v>
       </c>
       <c r="D25" s="9"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E25" s="9"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26" t="str">
         <v>CU-SAS002-P003</v>
       </c>
@@ -16983,8 +17014,9 @@
         <v>A2017</v>
       </c>
       <c r="D26" s="9"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E26" s="9"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A27" t="str">
         <v>CU-SAS003-P001</v>
       </c>
@@ -16997,8 +17029,9 @@
         <v>AR-M2</v>
       </c>
       <c r="D27" s="9"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E27" s="9"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A28" t="str">
         <v>CU-SAS003-P002</v>
       </c>
@@ -17011,8 +17044,9 @@
         <v>AR-M2</v>
       </c>
       <c r="D28" s="9"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E28" s="9"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A29" t="str">
         <v>LS001-P001</v>
       </c>
@@ -17025,8 +17059,9 @@
         <v>AR-M2</v>
       </c>
       <c r="D29" s="9"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E29" s="9"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A30" t="str">
         <v>LS-P002</v>
       </c>
@@ -17039,8 +17074,9 @@
         <v>AR-M2</v>
       </c>
       <c r="D30" s="9"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E30" s="9"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A31" t="str">
         <v>LS-P003</v>
       </c>
@@ -17053,8 +17089,9 @@
         <v>AR-M2</v>
       </c>
       <c r="D31" s="9"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E31" s="9"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A32" t="str">
         <v>LS-P004</v>
       </c>
@@ -17067,8 +17104,9 @@
         <v>AR-M2</v>
       </c>
       <c r="D32" s="9"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E32" s="9"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A33" t="str">
         <v>LS-P005</v>
       </c>
@@ -17081,8 +17119,9 @@
         <v>AR-M2</v>
       </c>
       <c r="D33" s="9"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E33" s="9"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A34" t="str">
         <v>R-HL-P001</v>
       </c>
@@ -17095,8 +17134,9 @@
         <v>A2017</v>
       </c>
       <c r="D34" s="9"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E34" s="9"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A35" t="str">
         <v>R-HL-P002</v>
       </c>
@@ -17109,8 +17149,9 @@
         <v>A2017</v>
       </c>
       <c r="D35" s="9"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E35" s="9"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A36" t="str">
         <v>R-HL-P003</v>
       </c>
@@ -17123,8 +17164,9 @@
         <v>A2017</v>
       </c>
       <c r="D36" s="9"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E36" s="9"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A37" t="str">
         <v>R-HL-P005</v>
       </c>
@@ -17137,8 +17179,9 @@
         <v>AR-M2</v>
       </c>
       <c r="D37" s="9"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E37" s="9"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A38" t="str">
         <v>R-HL-P006</v>
       </c>
@@ -17151,8 +17194,9 @@
         <v>A2017</v>
       </c>
       <c r="D38" s="9"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E38" s="9"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A39" t="str">
         <v>R-HL-RAS-P001</v>
       </c>
@@ -17165,8 +17209,9 @@
         <v>A2017</v>
       </c>
       <c r="D39" s="9"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E39" s="9"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A40" t="str">
         <v>R-HL-RAS-P002</v>
       </c>
@@ -17179,8 +17224,9 @@
         <v>A2017</v>
       </c>
       <c r="D40" s="9"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E40" s="9"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A41" t="str">
         <v>R-HL-RAS-P003</v>
       </c>
@@ -17193,8 +17239,9 @@
         <v>AR-M2</v>
       </c>
       <c r="D41" s="9"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E41" s="9"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A42" t="str">
         <v>RL-P001</v>
       </c>
@@ -17207,8 +17254,9 @@
         <v>A2017</v>
       </c>
       <c r="D42" s="9"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E42" s="9"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A43" t="str">
         <v>RL-P002</v>
       </c>
@@ -17221,8 +17269,9 @@
         <v>AR-M2</v>
       </c>
       <c r="D43" s="9"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E43" s="9"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A44" t="str">
         <v>R-P001</v>
       </c>
@@ -17235,8 +17284,9 @@
         <v>A2017</v>
       </c>
       <c r="D44" s="9"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E44" s="9"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A45" t="str">
         <v>R-P002</v>
       </c>
@@ -17249,8 +17299,9 @@
         <v>A2017</v>
       </c>
       <c r="D45" s="9"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E45" s="9"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A46" t="str">
         <v>R-P003</v>
       </c>
@@ -17263,8 +17314,9 @@
         <v>AR-M2</v>
       </c>
       <c r="D46" s="9"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E46" s="9"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A47" t="str">
         <v>R-P004</v>
       </c>
@@ -17277,8 +17329,9 @@
         <v>A2017</v>
       </c>
       <c r="D47" s="9"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E47" s="9"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A48" t="str">
         <v>R-P005</v>
       </c>
@@ -17291,8 +17344,9 @@
         <v>AR-M2</v>
       </c>
       <c r="D48" s="9"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E48" s="9"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A49" t="str">
         <v>RR-HL-RAS-P001</v>
       </c>
@@ -17305,8 +17359,9 @@
         <v>AR-M2</v>
       </c>
       <c r="D49" s="9"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E49" s="9"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A50" t="str">
         <v>RR-P001</v>
       </c>
@@ -17319,8 +17374,9 @@
         <v>A2017</v>
       </c>
       <c r="D50" s="9"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E50" s="9"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A51" t="str">
         <v>RR-P002</v>
       </c>
@@ -17333,8 +17389,9 @@
         <v>ｴﾎﾟｷｼ樹脂(充填剤なし)</v>
       </c>
       <c r="D51" s="9"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E51" s="9"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A52" t="str">
         <v>R-SA001-P001</v>
       </c>
@@ -17347,8 +17404,9 @@
         <v>A2017</v>
       </c>
       <c r="D52" s="9"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E52" s="9"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A53" t="str">
         <v>R-SA001-P002</v>
       </c>
@@ -17361,8 +17419,9 @@
         <v>A2017</v>
       </c>
       <c r="D53" s="9"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E53" s="9"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A54" t="str">
         <v>R-SA001-P003</v>
       </c>
@@ -17375,8 +17434,9 @@
         <v>A2017</v>
       </c>
       <c r="D54" s="9"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E54" s="9"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A55" t="str">
         <v>レシーバ v1</v>
       </c>
@@ -17389,8 +17449,9 @@
         <v>0</v>
       </c>
       <c r="D55" s="9"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E55" s="9"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A56" t="str">
         <v>右足駆動回路v2</v>
       </c>
@@ -17403,8 +17464,9 @@
         <v>0</v>
       </c>
       <c r="D56" s="9"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E56" s="9"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A57" t="str">
         <v>左足駆動回路v2</v>
       </c>
@@ -17417,8 +17479,9 @@
         <v>0</v>
       </c>
       <c r="D57" s="9"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E57" s="9"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A58" t="str">
         <v>電子回路ユニット</v>
       </c>
@@ -17431,8 +17494,9 @@
         <v>0</v>
       </c>
       <c r="D58" s="9"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E58" s="9"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A59" t="str">
         <v>腕駆動回路v2</v>
       </c>
@@ -17445,6 +17509,7 @@
         <v>電力回路基板</v>
       </c>
       <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>

</xml_diff>

<commit_message>
add : CAM files
</commit_message>
<xml_diff>
--- a/機械設計/_BOM/BOM.xlsx
+++ b/機械設計/_BOM/BOM.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\GitHub\2022-KawasakiRobot\機械設計\_BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449B149F-FEF2-42DB-88EB-0FC5E14F5BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0FF3D8-1EE5-469B-83C3-60040B415E0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="13410" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{F6B6BD99-36AE-468F-8B2F-9AA042AEB062}"/>
+    <workbookView xWindow="-28920" yWindow="13410" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{51BB279E-1BC7-45A7-AA7F-95296003500B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$T$1</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2207" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2312" uniqueCount="386">
   <si>
     <t>種類</t>
   </si>
@@ -1176,6 +1177,180 @@
   </si>
   <si>
     <t>A2017-BP-80-25</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">	A2017-BP-46-20</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>φ45 t7</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>φ75 t19</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CAM_T2_1</t>
+  </si>
+  <si>
+    <t>CAM_T2_1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>60x60xt2</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>16x40xt8</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>φ27.5 t5</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CAM_T5_1</t>
+  </si>
+  <si>
+    <t>CAM_T5_1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>t5</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>φ27.5 t10</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CAM_CU-AAS002-P001</t>
+  </si>
+  <si>
+    <t>CAM_CU-AAS002-P001</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>110x50xt7</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CAM_T8_1</t>
+  </si>
+  <si>
+    <t>CAM_T8_1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CAM_T3_1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>t3</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>AGILISTA</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>t8</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CAM_T3_2</t>
+  </si>
+  <si>
+    <t>CAM_T3_2</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>手加工</t>
+    <rPh sb="0" eb="3">
+      <t>テカコウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>A2017-BP-50-100</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>φ48 t17</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CAM_CU-SAS002-P001</t>
+  </si>
+  <si>
+    <t>CAM_CU-SAS002-P001</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>t10</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CAM_T12_1</t>
+  </si>
+  <si>
+    <t>CAM_T12_1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>t12</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>t2</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CAM_T2_2</t>
+  </si>
+  <si>
+    <t>CAM_T2_2</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>340x130xt2</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CAM_T2_3</t>
+  </si>
+  <si>
+    <t>CAM_T2_3</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">	A5052P-KQ2-350-200-2</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>A2017P-KQ3-240-170-3</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CAM_CGA75-P001</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">	A2017P-KQ5-300-180-5</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">	A5052P-KQ2-200-200-2</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">	A2017P-KQ8-400-200-8</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">	A2017P-KQ12-150-100-12</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1286,7 +1461,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1328,6 +1503,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2754,12 +2932,11 @@
         <v>2</v>
       </c>
       <c r="I25" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
@@ -2798,12 +2975,11 @@
         <v>2</v>
       </c>
       <c r="I26" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
@@ -2842,12 +3018,11 @@
         <v>1</v>
       </c>
       <c r="I27" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
@@ -2894,12 +3069,11 @@
         <v>3</v>
       </c>
       <c r="I28" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
@@ -14092,7 +14266,7 @@
       </c>
       <c r="C22">
         <f>SUMIF(Sheet1!C:C,B22,Sheet1!J:J)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.4">
@@ -14105,7 +14279,7 @@
       </c>
       <c r="C23">
         <f>SUMIF(Sheet1!C:C,B23,Sheet1!J:J)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.4">
@@ -14118,7 +14292,7 @@
       </c>
       <c r="C24">
         <f>SUMIF(Sheet1!C:C,B24,Sheet1!J:J)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.4">
@@ -14131,7 +14305,7 @@
       </c>
       <c r="C25">
         <f>SUMIF(Sheet1!C:C,B25,Sheet1!J:J)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.4">
@@ -15675,9 +15849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1F7574-C968-489E-91DC-0C793DF8D9FA}">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -16596,22 +16768,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A131F5D-359C-447A-A38B-BF4A40019FE6}">
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="21.625" customWidth="1"/>
     <col min="2" max="2" width="27.375" customWidth="1"/>
-    <col min="3" max="3" width="12.875" customWidth="1"/>
-    <col min="4" max="4" width="15.125" customWidth="1"/>
-    <col min="5" max="8" width="8.75" customWidth="1"/>
+    <col min="3" max="3" width="6.875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="20.875" customWidth="1"/>
+    <col min="5" max="5" width="24.5" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="21.625" customWidth="1"/>
+    <col min="8" max="9" width="8.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.4">
       <c r="A1" s="13" t="s">
         <v>332</v>
       </c>
@@ -16619,25 +16792,28 @@
         <v>333</v>
       </c>
       <c r="C1" s="13" t="s">
+        <v>320</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>334</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>339</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>338</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>335</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>336</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" t="str" cm="1">
         <f t="array" ref="A2:A59">_xlfn._xlws.SORT(_xlfn._xlws.FILTER(Sheet2!B22:B79,Sheet2!B22:B79&lt;&gt;""))</f>
         <v>CGA75-P001</v>
@@ -16646,17 +16822,23 @@
         <f>_xlfn.XLOOKUP(A2,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>内接歯車機構躯体</v>
       </c>
-      <c r="C2" s="9" t="str">
+      <c r="C2" s="9">
+        <f>_xlfn.XLOOKUP(A2,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="9" t="str">
         <f>_xlfn.XLOOKUP(A2,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>340</v>
-      </c>
       <c r="E2" s="9"/>
-      <c r="F2" s="11"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="F2" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" t="str">
         <v>CGA75-P002</v>
       </c>
@@ -16664,14 +16846,23 @@
         <f>_xlfn.XLOOKUP(A3,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>出力板</v>
       </c>
-      <c r="C3" s="9" t="str">
+      <c r="C3" s="9">
+        <f>_xlfn.XLOOKUP(A3,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="9" t="str">
         <f>_xlfn.XLOOKUP(A3,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="F3" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" t="str">
         <v>CGA75-P003</v>
       </c>
@@ -16679,14 +16870,23 @@
         <f>_xlfn.XLOOKUP(A4,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>内歯車</v>
       </c>
-      <c r="C4" s="9" t="str">
+      <c r="C4" s="9">
+        <f>_xlfn.XLOOKUP(A4,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D4" s="9" t="str">
         <f>_xlfn.XLOOKUP(A4,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D4" s="9"/>
       <c r="E4" s="9"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="F4" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5" t="str">
         <v>CGA75-P004</v>
       </c>
@@ -16694,14 +16894,21 @@
         <f>_xlfn.XLOOKUP(A5,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>曲軸(歯車付き)</v>
       </c>
-      <c r="C5" s="9" t="str">
+      <c r="C5" s="9">
+        <f>_xlfn.XLOOKUP(A5,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D5" s="9" t="str">
         <f>_xlfn.XLOOKUP(A5,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>S45C</v>
       </c>
-      <c r="D5" s="9"/>
       <c r="E5" s="9"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="F5" s="9"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" t="str">
         <v>CGA75-RS380-4-P001</v>
       </c>
@@ -16709,14 +16916,23 @@
         <f>_xlfn.XLOOKUP(A6,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>腕電動機取付板</v>
       </c>
-      <c r="C6" s="9" t="str">
+      <c r="C6" s="9">
+        <f>_xlfn.XLOOKUP(A6,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D6" s="9" t="str">
         <f>_xlfn.XLOOKUP(A6,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D6" s="9"/>
       <c r="E6" s="9"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="F6" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7" t="str">
         <v>CGA75-RS380-4-P002</v>
       </c>
@@ -16724,14 +16940,23 @@
         <f>_xlfn.XLOOKUP(A7,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>腕機構回路放熱板</v>
       </c>
-      <c r="C7" s="9" t="str">
+      <c r="C7" s="9">
+        <f>_xlfn.XLOOKUP(A7,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="9" t="str">
         <f>_xlfn.XLOOKUP(A7,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D7" s="9"/>
       <c r="E7" s="9"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="F7" s="9" t="s">
+        <v>347</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" t="str">
         <v>CU-AAS001-P001</v>
       </c>
@@ -16739,14 +16964,23 @@
         <f>_xlfn.XLOOKUP(A8,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>中関節</v>
       </c>
-      <c r="C8" s="9" t="str">
+      <c r="C8" s="9">
+        <f>_xlfn.XLOOKUP(A8,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>2</v>
+      </c>
+      <c r="D8" s="9" t="str">
         <f>_xlfn.XLOOKUP(A8,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D8" s="9"/>
       <c r="E8" s="9"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="F8" s="9" t="s">
+        <v>351</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A9" t="str">
         <v>CU-AAS002-P001</v>
       </c>
@@ -16754,14 +16988,23 @@
         <f>_xlfn.XLOOKUP(A9,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>従動節根本軸</v>
       </c>
-      <c r="C9" s="9" t="str">
+      <c r="C9" s="9">
+        <f>_xlfn.XLOOKUP(A9,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>2</v>
+      </c>
+      <c r="D9" s="9" t="str">
         <f>_xlfn.XLOOKUP(A9,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D9" s="9"/>
       <c r="E9" s="9"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="F9" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10" t="str">
         <v>CU-AAS002-P002</v>
       </c>
@@ -16769,14 +17012,23 @@
         <f>_xlfn.XLOOKUP(A10,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>駆動節歯車付き</v>
       </c>
-      <c r="C10" s="9" t="str">
+      <c r="C10" s="9">
+        <f>_xlfn.XLOOKUP(A10,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="9" t="str">
         <f>_xlfn.XLOOKUP(A10,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D10" s="9"/>
       <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="F10" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11" t="str">
         <v>CU-AAS002-P003</v>
       </c>
@@ -16784,14 +17036,23 @@
         <f>_xlfn.XLOOKUP(A11,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>駆動節</v>
       </c>
-      <c r="C11" s="9" t="str">
+      <c r="C11" s="9">
+        <f>_xlfn.XLOOKUP(A11,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D11" s="9" t="str">
         <f>_xlfn.XLOOKUP(A11,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D11" s="9"/>
       <c r="E11" s="9"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="F11" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" t="str">
         <v>CU-AAS003L-P001</v>
       </c>
@@ -16799,14 +17060,23 @@
         <f>_xlfn.XLOOKUP(A12,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>従動節左</v>
       </c>
-      <c r="C12" s="9" t="str">
+      <c r="C12" s="9">
+        <f>_xlfn.XLOOKUP(A12,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D12" s="9" t="str">
         <f>_xlfn.XLOOKUP(A12,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D12" s="9"/>
       <c r="E12" s="9"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="F12" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" t="str">
         <v>CU-AAS003-P001</v>
       </c>
@@ -16814,14 +17084,23 @@
         <f>_xlfn.XLOOKUP(A13,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>ロッド先端</v>
       </c>
-      <c r="C13" s="9" t="str">
+      <c r="C13" s="9">
+        <f>_xlfn.XLOOKUP(A13,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>2</v>
+      </c>
+      <c r="D13" s="9" t="str">
         <f>_xlfn.XLOOKUP(A13,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D13" s="9"/>
       <c r="E13" s="9"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="F13" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" t="str">
         <v>CU-AAS003R-P001</v>
       </c>
@@ -16829,14 +17108,23 @@
         <f>_xlfn.XLOOKUP(A14,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>従動節右</v>
       </c>
-      <c r="C14" s="9" t="str">
+      <c r="C14" s="9">
+        <f>_xlfn.XLOOKUP(A14,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D14" s="9" t="str">
         <f>_xlfn.XLOOKUP(A14,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D14" s="9"/>
       <c r="E14" s="9"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="F14" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15" t="str">
         <v>CU-AAS-P001</v>
       </c>
@@ -16844,14 +17132,23 @@
         <f>_xlfn.XLOOKUP(A15,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>カウンターアーム</v>
       </c>
-      <c r="C15" s="9" t="str">
+      <c r="C15" s="9">
+        <f>_xlfn.XLOOKUP(A15,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D15" s="9" t="str">
         <f>_xlfn.XLOOKUP(A15,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D15" s="9"/>
       <c r="E15" s="9"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="F15" s="9" t="s">
+        <v>351</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" t="str">
         <v>CU-AAS-P002</v>
       </c>
@@ -16859,14 +17156,23 @@
         <f>_xlfn.XLOOKUP(A16,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>ﾐﾗｰカウンターアーム</v>
       </c>
-      <c r="C16" s="9" t="str">
+      <c r="C16" s="9">
+        <f>_xlfn.XLOOKUP(A16,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D16" s="9" t="str">
         <f>_xlfn.XLOOKUP(A16,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D16" s="9"/>
       <c r="E16" s="9"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F16" s="9" t="s">
+        <v>351</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" t="str">
         <v>CU-AAS-P003</v>
       </c>
@@ -16874,14 +17180,21 @@
         <f>_xlfn.XLOOKUP(A17,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>腕機構カバー</v>
       </c>
-      <c r="C17" s="9" t="str">
+      <c r="C17" s="9">
+        <f>_xlfn.XLOOKUP(A17,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D17" s="9" t="str">
         <f>_xlfn.XLOOKUP(A17,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>AR-M2</v>
       </c>
-      <c r="D17" s="9"/>
       <c r="E17" s="9"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F17" s="9"/>
+      <c r="G17" s="12" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" t="str">
         <v>CU-AAS-P004</v>
       </c>
@@ -16889,14 +17202,21 @@
         <f>_xlfn.XLOOKUP(A18,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>ﾐﾗｰ腕機構カバー</v>
       </c>
-      <c r="C18" s="9" t="str">
+      <c r="C18" s="9">
+        <f>_xlfn.XLOOKUP(A18,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D18" s="9" t="str">
         <f>_xlfn.XLOOKUP(A18,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>AR-M2</v>
       </c>
-      <c r="D18" s="9"/>
       <c r="E18" s="9"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F18" s="9"/>
+      <c r="G18" s="12" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" t="str">
         <v>CU-P001</v>
       </c>
@@ -16904,14 +17224,21 @@
         <f>_xlfn.XLOOKUP(A19,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>中央ユニット後方カバー</v>
       </c>
-      <c r="C19" s="9" t="str">
+      <c r="C19" s="9">
+        <f>_xlfn.XLOOKUP(A19,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D19" s="9" t="str">
         <f>_xlfn.XLOOKUP(A19,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>AR-M2</v>
       </c>
-      <c r="D19" s="9"/>
       <c r="E19" s="9"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F19" s="9"/>
+      <c r="G19" s="12" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" t="str">
         <v>CU-P002</v>
       </c>
@@ -16919,14 +17246,23 @@
         <f>_xlfn.XLOOKUP(A20,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>足駆動回路放熱板</v>
       </c>
-      <c r="C20" s="9" t="str">
+      <c r="C20" s="9">
+        <f>_xlfn.XLOOKUP(A20,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D20" s="9" t="str">
         <f>_xlfn.XLOOKUP(A20,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D20" s="9"/>
       <c r="E20" s="9"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F20" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" t="str">
         <v>CU-SAS001-P001</v>
       </c>
@@ -16934,14 +17270,25 @@
         <f>_xlfn.XLOOKUP(A21,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>中央フレーム</v>
       </c>
-      <c r="C21" s="9" t="str">
+      <c r="C21" s="9">
+        <f>_xlfn.XLOOKUP(A21,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D21" s="9" t="str">
         <f>_xlfn.XLOOKUP(A21,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E21" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" t="str">
         <v>CU-SAS001-P002</v>
       </c>
@@ -16949,14 +17296,23 @@
         <f>_xlfn.XLOOKUP(A22,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>横展開抜止め</v>
       </c>
-      <c r="C22" s="9" t="str">
+      <c r="C22" s="9">
+        <f>_xlfn.XLOOKUP(A22,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>2</v>
+      </c>
+      <c r="D22" s="9" t="str">
         <f>_xlfn.XLOOKUP(A22,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D22" s="9"/>
       <c r="E22" s="9"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F22" s="9" t="s">
+        <v>351</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" t="str">
         <v>CU-SAS001-P003</v>
       </c>
@@ -16964,14 +17320,21 @@
         <f>_xlfn.XLOOKUP(A23,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>中央ユニット主軸</v>
       </c>
-      <c r="C23" s="9" t="str">
+      <c r="C23" s="9">
+        <f>_xlfn.XLOOKUP(A23,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D23" s="9" t="str">
         <f>_xlfn.XLOOKUP(A23,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D23" s="9"/>
       <c r="E23" s="9"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F23" s="9"/>
+      <c r="G23" s="12" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" t="str">
         <v>CU-SAS002-P001</v>
       </c>
@@ -16979,14 +17342,25 @@
         <f>_xlfn.XLOOKUP(A24,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>最集段ピニオン</v>
       </c>
-      <c r="C24" s="9" t="str">
+      <c r="C24" s="9">
+        <f>_xlfn.XLOOKUP(A24,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D24" s="9" t="str">
         <f>_xlfn.XLOOKUP(A24,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E24" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25" t="str">
         <v>CU-SAS002-P002</v>
       </c>
@@ -16994,14 +17368,23 @@
         <f>_xlfn.XLOOKUP(A25,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>腕機構内壁</v>
       </c>
-      <c r="C25" s="9" t="str">
+      <c r="C25" s="9">
+        <f>_xlfn.XLOOKUP(A25,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D25" s="9" t="str">
         <f>_xlfn.XLOOKUP(A25,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D25" s="9"/>
       <c r="E25" s="9"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F25" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A26" t="str">
         <v>CU-SAS002-P003</v>
       </c>
@@ -17009,14 +17392,23 @@
         <f>_xlfn.XLOOKUP(A26,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>腕機構内壁</v>
       </c>
-      <c r="C26" s="9" t="str">
+      <c r="C26" s="9">
+        <f>_xlfn.XLOOKUP(A26,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D26" s="9" t="str">
         <f>_xlfn.XLOOKUP(A26,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D26" s="9"/>
       <c r="E26" s="9"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F26" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A27" t="str">
         <v>CU-SAS003-P001</v>
       </c>
@@ -17024,14 +17416,21 @@
         <f>_xlfn.XLOOKUP(A27,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>抑制鍵</v>
       </c>
-      <c r="C27" s="9" t="str">
+      <c r="C27" s="9">
+        <f>_xlfn.XLOOKUP(A27,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D27" s="9" t="str">
         <f>_xlfn.XLOOKUP(A27,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>AR-M2</v>
       </c>
-      <c r="D27" s="9"/>
       <c r="E27" s="9"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F27" s="9"/>
+      <c r="G27" s="12" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A28" t="str">
         <v>CU-SAS003-P002</v>
       </c>
@@ -17039,14 +17438,21 @@
         <f>_xlfn.XLOOKUP(A28,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>展開機構ブロック</v>
       </c>
-      <c r="C28" s="9" t="str">
+      <c r="C28" s="9">
+        <f>_xlfn.XLOOKUP(A28,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D28" s="9" t="str">
         <f>_xlfn.XLOOKUP(A28,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>AR-M2</v>
       </c>
-      <c r="D28" s="9"/>
       <c r="E28" s="9"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F28" s="9"/>
+      <c r="G28" s="12" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A29" t="str">
         <v>LS001-P001</v>
       </c>
@@ -17054,14 +17460,21 @@
         <f>_xlfn.XLOOKUP(A29,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>リンクサス足側軸部</v>
       </c>
-      <c r="C29" s="9" t="str">
+      <c r="C29" s="9">
+        <f>_xlfn.XLOOKUP(A29,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D29" s="9" t="str">
         <f>_xlfn.XLOOKUP(A29,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>AR-M2</v>
       </c>
-      <c r="D29" s="9"/>
       <c r="E29" s="9"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F29" s="9"/>
+      <c r="G29" s="12" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A30" t="str">
         <v>LS-P002</v>
       </c>
@@ -17069,14 +17482,21 @@
         <f>_xlfn.XLOOKUP(A30,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>リンクサス長辺</v>
       </c>
-      <c r="C30" s="9" t="str">
+      <c r="C30" s="9">
+        <f>_xlfn.XLOOKUP(A30,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>2</v>
+      </c>
+      <c r="D30" s="9" t="str">
         <f>_xlfn.XLOOKUP(A30,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>AR-M2</v>
       </c>
-      <c r="D30" s="9"/>
       <c r="E30" s="9"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F30" s="9"/>
+      <c r="G30" s="12" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A31" t="str">
         <v>LS-P003</v>
       </c>
@@ -17084,14 +17504,21 @@
         <f>_xlfn.XLOOKUP(A31,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>リンクサス短辺</v>
       </c>
-      <c r="C31" s="9" t="str">
+      <c r="C31" s="9">
+        <f>_xlfn.XLOOKUP(A31,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>2</v>
+      </c>
+      <c r="D31" s="9" t="str">
         <f>_xlfn.XLOOKUP(A31,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>AR-M2</v>
       </c>
-      <c r="D31" s="9"/>
       <c r="E31" s="9"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F31" s="9"/>
+      <c r="G31" s="12" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A32" t="str">
         <v>LS-P004</v>
       </c>
@@ -17099,14 +17526,21 @@
         <f>_xlfn.XLOOKUP(A32,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>リンクサス中央軸部</v>
       </c>
-      <c r="C32" s="9" t="str">
+      <c r="C32" s="9">
+        <f>_xlfn.XLOOKUP(A32,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D32" s="9" t="str">
         <f>_xlfn.XLOOKUP(A32,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>AR-M2</v>
       </c>
-      <c r="D32" s="9"/>
       <c r="E32" s="9"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F32" s="9"/>
+      <c r="G32" s="12" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A33" t="str">
         <v>LS-P005</v>
       </c>
@@ -17114,14 +17548,21 @@
         <f>_xlfn.XLOOKUP(A33,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>リンクサス節軸</v>
       </c>
-      <c r="C33" s="9" t="str">
+      <c r="C33" s="9">
+        <f>_xlfn.XLOOKUP(A33,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>3</v>
+      </c>
+      <c r="D33" s="9" t="str">
         <f>_xlfn.XLOOKUP(A33,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>AR-M2</v>
       </c>
-      <c r="D33" s="9"/>
       <c r="E33" s="9"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F33" s="9"/>
+      <c r="G33" s="12" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A34" t="str">
         <v>R-HL-P001</v>
       </c>
@@ -17129,14 +17570,23 @@
         <f>_xlfn.XLOOKUP(A34,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>足曲軸長偏心体</v>
       </c>
-      <c r="C34" s="9" t="str">
+      <c r="C34" s="9">
+        <f>_xlfn.XLOOKUP(A34,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>8</v>
+      </c>
+      <c r="D34" s="9" t="str">
         <f>_xlfn.XLOOKUP(A34,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D34" s="9"/>
       <c r="E34" s="9"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F34" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A35" t="str">
         <v>R-HL-P002</v>
       </c>
@@ -17144,14 +17594,23 @@
         <f>_xlfn.XLOOKUP(A35,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>足曲軸短偏心体</v>
       </c>
-      <c r="C35" s="9" t="str">
+      <c r="C35" s="9">
+        <f>_xlfn.XLOOKUP(A35,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>4</v>
+      </c>
+      <c r="D35" s="9" t="str">
         <f>_xlfn.XLOOKUP(A35,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D35" s="9"/>
       <c r="E35" s="9"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F35" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A36" t="str">
         <v>R-HL-P003</v>
       </c>
@@ -17159,14 +17618,21 @@
         <f>_xlfn.XLOOKUP(A36,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>足プーリー中心軸</v>
       </c>
-      <c r="C36" s="9" t="str">
+      <c r="C36" s="9">
+        <f>_xlfn.XLOOKUP(A36,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>8</v>
+      </c>
+      <c r="D36" s="9" t="str">
         <f>_xlfn.XLOOKUP(A36,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D36" s="9"/>
       <c r="E36" s="9"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F36" s="9"/>
+      <c r="G36" s="12" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A37" t="str">
         <v>R-HL-P005</v>
       </c>
@@ -17174,14 +17640,21 @@
         <f>_xlfn.XLOOKUP(A37,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>ヘッケンリンク駆動プーリー</v>
       </c>
-      <c r="C37" s="9" t="str">
+      <c r="C37" s="9">
+        <f>_xlfn.XLOOKUP(A37,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>16</v>
+      </c>
+      <c r="D37" s="9" t="str">
         <f>_xlfn.XLOOKUP(A37,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>AR-M2</v>
       </c>
-      <c r="D37" s="9"/>
       <c r="E37" s="9"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F37" s="9"/>
+      <c r="G37" s="12" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A38" t="str">
         <v>R-HL-P006</v>
       </c>
@@ -17189,14 +17662,25 @@
         <f>_xlfn.XLOOKUP(A38,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>足プーリーフランジ</v>
       </c>
-      <c r="C38" s="9" t="str">
+      <c r="C38" s="9">
+        <f>_xlfn.XLOOKUP(A38,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>4</v>
+      </c>
+      <c r="D38" s="9" t="str">
         <f>_xlfn.XLOOKUP(A38,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E38" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A39" t="str">
         <v>R-HL-RAS-P001</v>
       </c>
@@ -17204,14 +17688,23 @@
         <f>_xlfn.XLOOKUP(A39,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>足上部</v>
       </c>
-      <c r="C39" s="9" t="str">
+      <c r="C39" s="9">
+        <f>_xlfn.XLOOKUP(A39,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>12</v>
+      </c>
+      <c r="D39" s="9" t="str">
         <f>_xlfn.XLOOKUP(A39,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D39" s="9"/>
       <c r="E39" s="9"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F39" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A40" t="str">
         <v>R-HL-RAS-P002</v>
       </c>
@@ -17219,14 +17712,23 @@
         <f>_xlfn.XLOOKUP(A40,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>足下部</v>
       </c>
-      <c r="C40" s="9" t="str">
+      <c r="C40" s="9">
+        <f>_xlfn.XLOOKUP(A40,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>12</v>
+      </c>
+      <c r="D40" s="9" t="str">
         <f>_xlfn.XLOOKUP(A40,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D40" s="9"/>
       <c r="E40" s="9"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F40" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A41" t="str">
         <v>R-HL-RAS-P003</v>
       </c>
@@ -17234,14 +17736,21 @@
         <f>_xlfn.XLOOKUP(A41,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>足ゴム</v>
       </c>
-      <c r="C41" s="9" t="str">
+      <c r="C41" s="9">
+        <f>_xlfn.XLOOKUP(A41,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>12</v>
+      </c>
+      <c r="D41" s="9" t="str">
         <f>_xlfn.XLOOKUP(A41,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>AR-M2</v>
       </c>
-      <c r="D41" s="9"/>
       <c r="E41" s="9"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F41" s="9"/>
+      <c r="G41" s="12" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A42" t="str">
         <v>RL-P001</v>
       </c>
@@ -17249,14 +17758,25 @@
         <f>_xlfn.XLOOKUP(A42,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>足側板左外側</v>
       </c>
-      <c r="C42" s="9" t="str">
+      <c r="C42" s="9">
+        <f>_xlfn.XLOOKUP(A42,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D42" s="9" t="str">
         <f>_xlfn.XLOOKUP(A42,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E42" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A43" t="str">
         <v>RL-P002</v>
       </c>
@@ -17264,14 +17784,21 @@
         <f>_xlfn.XLOOKUP(A43,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>左足機構側面充填樹脂</v>
       </c>
-      <c r="C43" s="9" t="str">
+      <c r="C43" s="9">
+        <f>_xlfn.XLOOKUP(A43,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D43" s="9" t="str">
         <f>_xlfn.XLOOKUP(A43,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>AR-M2</v>
       </c>
-      <c r="D43" s="9"/>
       <c r="E43" s="9"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F43" s="9"/>
+      <c r="G43" s="12" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A44" t="str">
         <v>R-P001</v>
       </c>
@@ -17279,14 +17806,25 @@
         <f>_xlfn.XLOOKUP(A44,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>足側板内側</v>
       </c>
-      <c r="C44" s="9" t="str">
+      <c r="C44" s="9">
+        <f>_xlfn.XLOOKUP(A44,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>2</v>
+      </c>
+      <c r="D44" s="9" t="str">
         <f>_xlfn.XLOOKUP(A44,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E44" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="G44" s="11" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A45" t="str">
         <v>R-P002</v>
       </c>
@@ -17294,14 +17832,21 @@
         <f>_xlfn.XLOOKUP(A45,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>足機構固定板</v>
       </c>
-      <c r="C45" s="9" t="str">
+      <c r="C45" s="9">
+        <f>_xlfn.XLOOKUP(A45,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>2</v>
+      </c>
+      <c r="D45" s="9" t="str">
         <f>_xlfn.XLOOKUP(A45,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D45" s="9"/>
       <c r="E45" s="9"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F45" s="9"/>
+      <c r="G45" s="11" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A46" t="str">
         <v>R-P003</v>
       </c>
@@ -17309,14 +17854,21 @@
         <f>_xlfn.XLOOKUP(A46,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>足機構上面カバー</v>
       </c>
-      <c r="C46" s="9" t="str">
+      <c r="C46" s="9">
+        <f>_xlfn.XLOOKUP(A46,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>2</v>
+      </c>
+      <c r="D46" s="9" t="str">
         <f>_xlfn.XLOOKUP(A46,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>AR-M2</v>
       </c>
-      <c r="D46" s="9"/>
       <c r="E46" s="9"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F46" s="9"/>
+      <c r="G46" s="12" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A47" t="str">
         <v>R-P004</v>
       </c>
@@ -17324,14 +17876,21 @@
         <f>_xlfn.XLOOKUP(A47,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>足機構主柱</v>
       </c>
-      <c r="C47" s="9" t="str">
+      <c r="C47" s="9">
+        <f>_xlfn.XLOOKUP(A47,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>8</v>
+      </c>
+      <c r="D47" s="9" t="str">
         <f>_xlfn.XLOOKUP(A47,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D47" s="9"/>
       <c r="E47" s="9"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F47" s="9"/>
+      <c r="G47" s="12" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A48" t="str">
         <v>R-P005</v>
       </c>
@@ -17339,14 +17898,21 @@
         <f>_xlfn.XLOOKUP(A48,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>カウンターアームロック</v>
       </c>
-      <c r="C48" s="9" t="str">
+      <c r="C48" s="9">
+        <f>_xlfn.XLOOKUP(A48,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>2</v>
+      </c>
+      <c r="D48" s="9" t="str">
         <f>_xlfn.XLOOKUP(A48,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>AR-M2</v>
       </c>
-      <c r="D48" s="9"/>
       <c r="E48" s="9"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F48" s="9"/>
+      <c r="G48" s="12" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A49" t="str">
         <v>RR-HL-RAS-P001</v>
       </c>
@@ -17354,14 +17920,21 @@
         <f>_xlfn.XLOOKUP(A49,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>前足底左半身側</v>
       </c>
-      <c r="C49" s="9" t="str">
+      <c r="C49" s="9">
+        <f>_xlfn.XLOOKUP(A49,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>12</v>
+      </c>
+      <c r="D49" s="9" t="str">
         <f>_xlfn.XLOOKUP(A49,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>AR-M2</v>
       </c>
-      <c r="D49" s="9"/>
       <c r="E49" s="9"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F49" s="9"/>
+      <c r="G49" s="12" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A50" t="str">
         <v>RR-P001</v>
       </c>
@@ -17369,14 +17942,25 @@
         <f>_xlfn.XLOOKUP(A50,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>足側板右外側</v>
       </c>
-      <c r="C50" s="9" t="str">
+      <c r="C50" s="9">
+        <f>_xlfn.XLOOKUP(A50,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D50" s="9" t="str">
         <f>_xlfn.XLOOKUP(A50,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E50" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="G50" s="11" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A51" t="str">
         <v>RR-P002</v>
       </c>
@@ -17384,14 +17968,21 @@
         <f>_xlfn.XLOOKUP(A51,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>右足機構側面充填樹脂</v>
       </c>
-      <c r="C51" s="9" t="str">
+      <c r="C51" s="9">
+        <f>_xlfn.XLOOKUP(A51,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D51" s="9" t="str">
         <f>_xlfn.XLOOKUP(A51,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>ｴﾎﾟｷｼ樹脂(充填剤なし)</v>
       </c>
-      <c r="D51" s="9"/>
       <c r="E51" s="9"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F51" s="9"/>
+      <c r="G51" s="12" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A52" t="str">
         <v>R-SA001-P001</v>
       </c>
@@ -17399,14 +17990,21 @@
         <f>_xlfn.XLOOKUP(A52,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>足中間歯車1A</v>
       </c>
-      <c r="C52" s="9" t="str">
+      <c r="C52" s="9">
+        <f>_xlfn.XLOOKUP(A52,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>2</v>
+      </c>
+      <c r="D52" s="9" t="str">
         <f>_xlfn.XLOOKUP(A52,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D52" s="9"/>
       <c r="E52" s="9"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F52" s="9"/>
+      <c r="G52" s="11" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A53" t="str">
         <v>R-SA001-P002</v>
       </c>
@@ -17414,14 +18012,21 @@
         <f>_xlfn.XLOOKUP(A53,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>足中間歯車1B</v>
       </c>
-      <c r="C53" s="9" t="str">
+      <c r="C53" s="9">
+        <f>_xlfn.XLOOKUP(A53,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>2</v>
+      </c>
+      <c r="D53" s="9" t="str">
         <f>_xlfn.XLOOKUP(A53,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D53" s="9"/>
       <c r="E53" s="9"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F53" s="9"/>
+      <c r="G53" s="11" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A54" t="str">
         <v>R-SA001-P003</v>
       </c>
@@ -17429,14 +18034,19 @@
         <f>_xlfn.XLOOKUP(A54,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>足中間歯車2</v>
       </c>
-      <c r="C54" s="9" t="str">
+      <c r="C54" s="9">
+        <f>_xlfn.XLOOKUP(A54,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>2</v>
+      </c>
+      <c r="D54" s="9" t="str">
         <f>_xlfn.XLOOKUP(A54,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>A2017</v>
       </c>
-      <c r="D54" s="9"/>
       <c r="E54" s="9"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F54" s="9"/>
+      <c r="G54" s="11"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A55" t="str">
         <v>レシーバ v1</v>
       </c>
@@ -17445,13 +18055,17 @@
         <v>レシーバ v1</v>
       </c>
       <c r="C55" s="9">
+        <f>_xlfn.XLOOKUP(A55,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D55" s="9">
         <f>_xlfn.XLOOKUP(A55,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>0</v>
       </c>
-      <c r="D55" s="9"/>
       <c r="E55" s="9"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F55" s="9"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A56" t="str">
         <v>右足駆動回路v2</v>
       </c>
@@ -17460,13 +18074,17 @@
         <v>右足駆動回路v2</v>
       </c>
       <c r="C56" s="9">
+        <f>_xlfn.XLOOKUP(A56,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D56" s="9">
         <f>_xlfn.XLOOKUP(A56,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>0</v>
       </c>
-      <c r="D56" s="9"/>
       <c r="E56" s="9"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F56" s="9"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A57" t="str">
         <v>左足駆動回路v2</v>
       </c>
@@ -17475,13 +18093,17 @@
         <v>左足駆動回路v2</v>
       </c>
       <c r="C57" s="9">
+        <f>_xlfn.XLOOKUP(A57,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D57" s="9">
         <f>_xlfn.XLOOKUP(A57,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>0</v>
       </c>
-      <c r="D57" s="9"/>
       <c r="E57" s="9"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F57" s="9"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A58" t="str">
         <v>電子回路ユニット</v>
       </c>
@@ -17490,13 +18112,17 @@
         <v>電子回路ユニット</v>
       </c>
       <c r="C58" s="9">
+        <f>_xlfn.XLOOKUP(A58,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D58" s="9">
         <f>_xlfn.XLOOKUP(A58,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>0</v>
       </c>
-      <c r="D58" s="9"/>
       <c r="E58" s="9"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F58" s="9"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A59" t="str">
         <v>腕駆動回路v2</v>
       </c>
@@ -17504,12 +18130,181 @@
         <f>_xlfn.XLOOKUP(A59,Sheet1!$C:$C,Sheet1!$F:$F)</f>
         <v>腕駆動回路v2</v>
       </c>
-      <c r="C59" s="9" t="str">
+      <c r="C59" s="9">
+        <f>_xlfn.XLOOKUP(A59,Sheet2!$B:$B,Sheet2!$C:$C)</f>
+        <v>1</v>
+      </c>
+      <c r="D59" s="9" t="str">
         <f>_xlfn.XLOOKUP(A59,Sheet1!$C:$C,Sheet1!$G:$G)</f>
         <v>電力回路基板</v>
       </c>
-      <c r="D59" s="9"/>
       <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F332DD2-F615-4383-B5E3-0355B0E5BFED}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E9" sqref="D1:E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="25.375" style="14" customWidth="1"/>
+    <col min="4" max="4" width="33.5" style="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>340</v>
+      </c>
+      <c r="D1" s="14" t="str" cm="1">
+        <f t="array" ref="D1:D9">_xlfn.UNIQUE(_xlfn._xlws.SORT(_xlfn._xlws.FILTER(B:B,B:B&lt;&gt;"")))</f>
+        <v xml:space="preserve">	A2017-BP-46-20</v>
+      </c>
+      <c r="E1">
+        <f>COUNTIF(B:B,D1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>341</v>
+      </c>
+      <c r="D2" s="14" t="str">
+        <v xml:space="preserve">	A2017P-KQ12-150-100-12</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E9" si="0">COUNTIF(B:B,D2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>367</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>365</v>
+      </c>
+      <c r="D3" s="14" t="str">
+        <v xml:space="preserve">	A2017P-KQ5-300-180-5</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>344</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>383</v>
+      </c>
+      <c r="D4" s="14" t="str">
+        <v xml:space="preserve">	A2017P-KQ8-400-200-8</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>374</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5" s="14" t="str">
+        <v xml:space="preserve">	A5052P-KQ2-200-200-2</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>377</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="D6" s="14" t="str">
+        <v xml:space="preserve">	A5052P-KQ2-350-200-2</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>362</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>380</v>
+      </c>
+      <c r="D7" s="14" t="str">
+        <v>A2017-BP-50-100</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>349</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>382</v>
+      </c>
+      <c r="D8" s="14" t="str">
+        <v>A2017-BP-80-25</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>356</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>384</v>
+      </c>
+      <c r="D9" s="14" t="str">
+        <v>A2017P-KQ3-240-170-3</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>370</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>385</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>

</xml_diff>

<commit_message>
point : make comp
</commit_message>
<xml_diff>
--- a/機械設計/_BOM/BOM.xlsx
+++ b/機械設計/_BOM/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\GitHub\2022-KawasakiRobot\機械設計\_BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E1CE61-B7F6-4F86-ABEF-96E2E044E603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F389EB39-7A60-494A-98DD-2FB4DFD6BE87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{51BB279E-1BC7-45A7-AA7F-95296003500B}"/>
+    <workbookView xWindow="-28920" yWindow="-2790" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{51BB279E-1BC7-45A7-AA7F-95296003500B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1838,7 +1838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B61C4854-7AE2-455B-B515-BBA850988212}">
   <dimension ref="A1:T241"/>
   <sheetViews>
-    <sheetView topLeftCell="A226" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A184" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A242" sqref="A242:XFD245"/>
     </sheetView>
   </sheetViews>
@@ -2077,7 +2077,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="5">
-        <f>SUMIF($C:$C,"="&amp;B5,J:J)</f>
+        <f t="shared" ref="I5:I24" si="1">SUMIF($C:$C,"="&amp;B5,J:J)</f>
         <v>1</v>
       </c>
       <c r="J5" s="5">
@@ -2121,7 +2121,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="5">
-        <f>SUMIF($C:$C,"="&amp;B6,J:J)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J6" s="5">
@@ -2163,7 +2163,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="5">
-        <f>SUMIF($C:$C,"="&amp;B7,J:J)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J7" s="5">
@@ -2207,7 +2207,7 @@
         <v>1</v>
       </c>
       <c r="I8" s="5">
-        <f>SUMIF($C:$C,"="&amp;B8,J:J)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J8" s="5">
@@ -2249,7 +2249,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="5">
-        <f>SUMIF($C:$C,"="&amp;B9,J:J)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J9" s="5">
@@ -2291,7 +2291,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="5">
-        <f>SUMIF($C:$C,"="&amp;B10,J:J)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J10" s="5">
@@ -2333,7 +2333,7 @@
         <v>1</v>
       </c>
       <c r="I11" s="5">
-        <f>SUMIF($C:$C,"="&amp;B11,J:J)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J11" s="5">
@@ -2375,7 +2375,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="5">
-        <f>SUMIF($C:$C,"="&amp;B12,J:J)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J12" s="5">
@@ -2417,7 +2417,7 @@
         <v>1</v>
       </c>
       <c r="I13" s="5">
-        <f>SUMIF($C:$C,"="&amp;B13,J:J)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J13" s="5">
@@ -2461,7 +2461,7 @@
         <v>1</v>
       </c>
       <c r="I14" s="5">
-        <f>SUMIF($C:$C,"="&amp;B14,J:J)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J14" s="5">
@@ -2505,7 +2505,7 @@
         <v>1</v>
       </c>
       <c r="I15" s="5">
-        <f>SUMIF($C:$C,"="&amp;B15,J:J)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J15" s="5">
@@ -2549,7 +2549,7 @@
         <v>3</v>
       </c>
       <c r="I16" s="5">
-        <f>SUMIF($C:$C,"="&amp;B16,J:J)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J16" s="5">
@@ -2593,7 +2593,7 @@
         <v>3</v>
       </c>
       <c r="I17" s="5">
-        <f>SUMIF($C:$C,"="&amp;B17,J:J)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J17" s="5">
@@ -2637,7 +2637,7 @@
         <v>1</v>
       </c>
       <c r="I18" s="5">
-        <f>SUMIF($C:$C,"="&amp;B18,J:J)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J18" s="5">
@@ -2681,7 +2681,7 @@
         <v>1</v>
       </c>
       <c r="I19" s="5">
-        <f>SUMIF($C:$C,"="&amp;B19,J:J)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J19" s="5">
@@ -2725,7 +2725,7 @@
         <v>1</v>
       </c>
       <c r="I20" s="5">
-        <f>SUMIF($C:$C,"="&amp;B20,J:J)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J20" s="5">
@@ -2769,7 +2769,7 @@
         <v>3</v>
       </c>
       <c r="I21" s="5">
-        <f>SUMIF($C:$C,"="&amp;B21,J:J)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J21" s="5">
@@ -2813,7 +2813,7 @@
         <v>3</v>
       </c>
       <c r="I22" s="5">
-        <f>SUMIF($C:$C,"="&amp;B22,J:J)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J22" s="5">
@@ -2857,7 +2857,7 @@
         <v>1</v>
       </c>
       <c r="I23" s="5">
-        <f>SUMIF($C:$C,"="&amp;B23,J:J)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J23" s="5">
@@ -2901,7 +2901,7 @@
         <v>1</v>
       </c>
       <c r="I24" s="5">
-        <f>SUMIF($C:$C,"="&amp;B24,J:J)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J24" s="5">
@@ -3135,7 +3135,7 @@
         <v>1</v>
       </c>
       <c r="I29" s="5">
-        <f>SUMIF($C:$C,"="&amp;B29,J:J)</f>
+        <f t="shared" ref="I29:I92" si="2">SUMIF($C:$C,"="&amp;B29,J:J)</f>
         <v>1</v>
       </c>
       <c r="J29" s="5">
@@ -3185,7 +3185,7 @@
         <v>1</v>
       </c>
       <c r="I30" s="5">
-        <f>SUMIF($C:$C,"="&amp;B30,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J30" s="5">
@@ -3235,7 +3235,7 @@
         <v>1</v>
       </c>
       <c r="I31" s="5">
-        <f>SUMIF($C:$C,"="&amp;B31,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J31" s="5">
@@ -3277,7 +3277,7 @@
         <v>2</v>
       </c>
       <c r="I32" s="5">
-        <f>SUMIF($C:$C,"="&amp;B32,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J32" s="5">
@@ -3319,7 +3319,7 @@
         <v>1</v>
       </c>
       <c r="I33" s="5">
-        <f>SUMIF($C:$C,"="&amp;B33,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J33" s="5">
@@ -3363,7 +3363,7 @@
         <v>1</v>
       </c>
       <c r="I34" s="5">
-        <f>SUMIF($C:$C,"="&amp;B34,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J34" s="5">
@@ -3409,7 +3409,7 @@
         <v>1</v>
       </c>
       <c r="I35" s="5">
-        <f>SUMIF($C:$C,"="&amp;B35,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J35" s="5">
@@ -3455,7 +3455,7 @@
         <v>1</v>
       </c>
       <c r="I36" s="5">
-        <f>SUMIF($C:$C,"="&amp;B36,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J36" s="5">
@@ -3501,7 +3501,7 @@
         <v>1</v>
       </c>
       <c r="I37" s="5">
-        <f>SUMIF($C:$C,"="&amp;B37,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J37" s="5">
@@ -3547,7 +3547,7 @@
         <v>1</v>
       </c>
       <c r="I38" s="5">
-        <f>SUMIF($C:$C,"="&amp;B38,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J38" s="5">
@@ -3593,7 +3593,7 @@
         <v>1</v>
       </c>
       <c r="I39" s="5">
-        <f>SUMIF($C:$C,"="&amp;B39,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J39" s="5">
@@ -3639,7 +3639,7 @@
         <v>1</v>
       </c>
       <c r="I40" s="5">
-        <f>SUMIF($C:$C,"="&amp;B40,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J40" s="5">
@@ -3685,7 +3685,7 @@
         <v>1</v>
       </c>
       <c r="I41" s="5">
-        <f>SUMIF($C:$C,"="&amp;B41,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J41" s="5">
@@ -3733,7 +3733,7 @@
         <v>1</v>
       </c>
       <c r="I42" s="5">
-        <f>SUMIF($C:$C,"="&amp;B42,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J42" s="5">
@@ -3781,7 +3781,7 @@
         <v>2</v>
       </c>
       <c r="I43" s="5">
-        <f>SUMIF($C:$C,"="&amp;B43,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J43" s="5">
@@ -3825,7 +3825,7 @@
         <v>2</v>
       </c>
       <c r="I44" s="5">
-        <f>SUMIF($C:$C,"="&amp;B44,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J44" s="5">
@@ -3869,7 +3869,7 @@
         <v>1</v>
       </c>
       <c r="I45" s="5">
-        <f>SUMIF($C:$C,"="&amp;B45,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J45" s="5">
@@ -3913,7 +3913,7 @@
         <v>1</v>
       </c>
       <c r="I46" s="5">
-        <f>SUMIF($C:$C,"="&amp;B46,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J46" s="5">
@@ -3957,7 +3957,7 @@
         <v>1</v>
       </c>
       <c r="I47" s="5">
-        <f>SUMIF($C:$C,"="&amp;B47,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J47" s="5">
@@ -4009,7 +4009,7 @@
         <v>1</v>
       </c>
       <c r="I48" s="5">
-        <f>SUMIF($C:$C,"="&amp;B48,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J48" s="5">
@@ -4061,7 +4061,7 @@
         <v>1</v>
       </c>
       <c r="I49" s="5">
-        <f>SUMIF($C:$C,"="&amp;B49,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J49" s="5">
@@ -4113,7 +4113,7 @@
         <v>1</v>
       </c>
       <c r="I50" s="5">
-        <f>SUMIF($C:$C,"="&amp;B50,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J50" s="5">
@@ -4165,7 +4165,7 @@
         <v>1</v>
       </c>
       <c r="I51" s="5">
-        <f>SUMIF($C:$C,"="&amp;B51,J:J)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J51" s="5">
@@ -4217,7 +4217,7 @@
         <v>1</v>
       </c>
       <c r="I52" s="5">
-        <f>SUMIF($C:$C,"="&amp;B52,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J52" s="5">
@@ -4269,7 +4269,7 @@
         <v>1</v>
       </c>
       <c r="I53" s="5">
-        <f>SUMIF($C:$C,"="&amp;B53,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J53" s="5">
@@ -4321,7 +4321,7 @@
         <v>1</v>
       </c>
       <c r="I54" s="5">
-        <f>SUMIF($C:$C,"="&amp;B54,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J54" s="5">
@@ -4373,7 +4373,7 @@
         <v>4</v>
       </c>
       <c r="I55" s="5">
-        <f>SUMIF($C:$C,"="&amp;B55,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J55" s="5">
@@ -4425,7 +4425,7 @@
         <v>1</v>
       </c>
       <c r="I56" s="5">
-        <f>SUMIF($C:$C,"="&amp;B56,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J56" s="5">
@@ -4477,7 +4477,7 @@
         <v>1</v>
       </c>
       <c r="I57" s="5">
-        <f>SUMIF($C:$C,"="&amp;B57,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J57" s="5">
@@ -4529,7 +4529,7 @@
         <v>1</v>
       </c>
       <c r="I58" s="5">
-        <f>SUMIF($C:$C,"="&amp;B58,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J58" s="5">
@@ -4581,7 +4581,7 @@
         <v>2</v>
       </c>
       <c r="I59" s="5">
-        <f>SUMIF($C:$C,"="&amp;B59,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J59" s="5">
@@ -4625,7 +4625,7 @@
         <v>1</v>
       </c>
       <c r="I60" s="5">
-        <f>SUMIF($C:$C,"="&amp;B60,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J60" s="5">
@@ -4669,7 +4669,7 @@
         <v>1</v>
       </c>
       <c r="I61" s="5">
-        <f>SUMIF($C:$C,"="&amp;B61,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J61" s="5">
@@ -4721,7 +4721,7 @@
         <v>1</v>
       </c>
       <c r="I62" s="5">
-        <f>SUMIF($C:$C,"="&amp;B62,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J62" s="5">
@@ -4765,7 +4765,7 @@
         <v>1</v>
       </c>
       <c r="I63" s="5">
-        <f>SUMIF($C:$C,"="&amp;B63,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J63" s="5">
@@ -4817,7 +4817,7 @@
         <v>1</v>
       </c>
       <c r="I64" s="5">
-        <f>SUMIF($C:$C,"="&amp;B64,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J64" s="5">
@@ -4869,11 +4869,11 @@
         <v>3</v>
       </c>
       <c r="I65" s="5">
-        <f>SUMIF($C:$C,"="&amp;B65,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J65" s="5">
-        <f t="shared" ref="J65" si="1">H65*I65</f>
+        <f t="shared" ref="J65" si="3">H65*I65</f>
         <v>3</v>
       </c>
       <c r="K65" s="5"/>
@@ -4921,7 +4921,7 @@
         <v>2</v>
       </c>
       <c r="I66" s="5">
-        <f>SUMIF($C:$C,"="&amp;B66,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J66" s="5">
@@ -4965,11 +4965,11 @@
         <v>1</v>
       </c>
       <c r="I67" s="5">
-        <f>SUMIF($C:$C,"="&amp;B67,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J67" s="5">
-        <f t="shared" ref="J67:J133" si="2">H67*I67</f>
+        <f t="shared" ref="J67:J133" si="4">H67*I67</f>
         <v>1</v>
       </c>
       <c r="K67" s="5"/>
@@ -5009,11 +5009,11 @@
         <v>1</v>
       </c>
       <c r="I68" s="5">
-        <f>SUMIF($C:$C,"="&amp;B68,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J68" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K68" s="5"/>
@@ -5061,11 +5061,11 @@
         <v>1</v>
       </c>
       <c r="I69" s="5">
-        <f>SUMIF($C:$C,"="&amp;B69,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J69" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K69" s="5"/>
@@ -5105,11 +5105,11 @@
         <v>1</v>
       </c>
       <c r="I70" s="5">
-        <f>SUMIF($C:$C,"="&amp;B70,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J70" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K70" s="5"/>
@@ -5157,11 +5157,11 @@
         <v>1</v>
       </c>
       <c r="I71" s="5">
-        <f>SUMIF($C:$C,"="&amp;B71,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J71" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K71" s="5"/>
@@ -5209,11 +5209,11 @@
         <v>3</v>
       </c>
       <c r="I72" s="5">
-        <f>SUMIF($C:$C,"="&amp;B72,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J72" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="K72" s="5"/>
@@ -5261,11 +5261,11 @@
         <v>1</v>
       </c>
       <c r="I73" s="5">
-        <f>SUMIF($C:$C,"="&amp;B73,J:J)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="J73" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="K73" s="5"/>
@@ -5305,11 +5305,11 @@
         <v>1</v>
       </c>
       <c r="I74" s="5">
-        <f>SUMIF($C:$C,"="&amp;B74,J:J)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="J74" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="K74" s="5"/>
@@ -5349,11 +5349,11 @@
         <v>1</v>
       </c>
       <c r="I75" s="5">
-        <f>SUMIF($C:$C,"="&amp;B75,J:J)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="J75" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="K75" s="5"/>
@@ -5393,11 +5393,11 @@
         <v>1</v>
       </c>
       <c r="I76" s="5">
-        <f>SUMIF($C:$C,"="&amp;B76,J:J)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="J76" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="K76" s="5"/>
@@ -5437,11 +5437,11 @@
         <v>1</v>
       </c>
       <c r="I77" s="5">
-        <f>SUMIF($C:$C,"="&amp;B77,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J77" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K77" s="5"/>
@@ -5489,11 +5489,11 @@
         <v>1</v>
       </c>
       <c r="I78" s="5">
-        <f>SUMIF($C:$C,"="&amp;B78,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J78" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K78" s="5"/>
@@ -5541,11 +5541,11 @@
         <v>1</v>
       </c>
       <c r="I79" s="5">
-        <f>SUMIF($C:$C,"="&amp;B79,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J79" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K79" s="5"/>
@@ -5593,11 +5593,11 @@
         <v>1</v>
       </c>
       <c r="I80" s="5">
-        <f>SUMIF($C:$C,"="&amp;B80,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J80" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K80" s="5"/>
@@ -5645,11 +5645,11 @@
         <v>4</v>
       </c>
       <c r="I81" s="5">
-        <f>SUMIF($C:$C,"="&amp;B81,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J81" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="K81" s="5"/>
@@ -5697,11 +5697,11 @@
         <v>1</v>
       </c>
       <c r="I82" s="5">
-        <f>SUMIF($C:$C,"="&amp;B82,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J82" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K82" s="5"/>
@@ -5749,11 +5749,11 @@
         <v>1</v>
       </c>
       <c r="I83" s="5">
-        <f>SUMIF($C:$C,"="&amp;B83,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J83" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K83" s="5"/>
@@ -5801,11 +5801,11 @@
         <v>1</v>
       </c>
       <c r="I84" s="5">
-        <f>SUMIF($C:$C,"="&amp;B84,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J84" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K84" s="5"/>
@@ -5853,11 +5853,11 @@
         <v>2</v>
       </c>
       <c r="I85" s="5">
-        <f>SUMIF($C:$C,"="&amp;B85,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J85" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="K85" s="5"/>
@@ -5897,11 +5897,11 @@
         <v>1</v>
       </c>
       <c r="I86" s="5">
-        <f>SUMIF($C:$C,"="&amp;B86,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J86" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K86" s="5"/>
@@ -5941,11 +5941,11 @@
         <v>1</v>
       </c>
       <c r="I87" s="5">
-        <f>SUMIF($C:$C,"="&amp;B87,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J87" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K87" s="5"/>
@@ -5993,11 +5993,11 @@
         <v>1</v>
       </c>
       <c r="I88" s="5">
-        <f>SUMIF($C:$C,"="&amp;B88,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J88" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K88" s="5"/>
@@ -6037,7 +6037,7 @@
         <v>1</v>
       </c>
       <c r="I89" s="5">
-        <f>SUMIF($C:$C,"="&amp;B89,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J89" s="5">
@@ -6089,11 +6089,11 @@
         <v>1</v>
       </c>
       <c r="I90" s="5">
-        <f>SUMIF($C:$C,"="&amp;B90,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J90" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K90" s="5"/>
@@ -6141,11 +6141,11 @@
         <v>3</v>
       </c>
       <c r="I91" s="5">
-        <f>SUMIF($C:$C,"="&amp;B91,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J91" s="5">
-        <f t="shared" ref="J91" si="3">H91*I91</f>
+        <f t="shared" ref="J91" si="5">H91*I91</f>
         <v>3</v>
       </c>
       <c r="K91" s="5"/>
@@ -6193,11 +6193,11 @@
         <v>2</v>
       </c>
       <c r="I92" s="5">
-        <f>SUMIF($C:$C,"="&amp;B92,J:J)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J92" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="K92" s="5"/>
@@ -6237,11 +6237,11 @@
         <v>1</v>
       </c>
       <c r="I93" s="5">
-        <f>SUMIF($C:$C,"="&amp;B93,J:J)</f>
+        <f t="shared" ref="I93:I156" si="6">SUMIF($C:$C,"="&amp;B93,J:J)</f>
         <v>1</v>
       </c>
       <c r="J93" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K93" s="5"/>
@@ -6281,11 +6281,11 @@
         <v>1</v>
       </c>
       <c r="I94" s="5">
-        <f>SUMIF($C:$C,"="&amp;B94,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J94" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K94" s="5"/>
@@ -6333,11 +6333,11 @@
         <v>1</v>
       </c>
       <c r="I95" s="5">
-        <f>SUMIF($C:$C,"="&amp;B95,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J95" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K95" s="5"/>
@@ -6377,11 +6377,11 @@
         <v>1</v>
       </c>
       <c r="I96" s="5">
-        <f>SUMIF($C:$C,"="&amp;B96,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J96" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K96" s="5"/>
@@ -6429,11 +6429,11 @@
         <v>1</v>
       </c>
       <c r="I97" s="5">
-        <f>SUMIF($C:$C,"="&amp;B97,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J97" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K97" s="5"/>
@@ -6481,11 +6481,11 @@
         <v>3</v>
       </c>
       <c r="I98" s="5">
-        <f>SUMIF($C:$C,"="&amp;B98,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J98" s="5">
-        <f t="shared" ref="J98" si="4">H98*I98</f>
+        <f t="shared" ref="J98" si="7">H98*I98</f>
         <v>3</v>
       </c>
       <c r="K98" s="5"/>
@@ -6533,11 +6533,11 @@
         <v>1</v>
       </c>
       <c r="I99" s="5">
-        <f>SUMIF($C:$C,"="&amp;B99,J:J)</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="J99" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="K99" s="5"/>
@@ -6577,11 +6577,11 @@
         <v>1</v>
       </c>
       <c r="I100" s="5">
-        <f>SUMIF($C:$C,"="&amp;B100,J:J)</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="J100" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="K100" s="5"/>
@@ -6621,11 +6621,11 @@
         <v>1</v>
       </c>
       <c r="I101" s="5">
-        <f>SUMIF($C:$C,"="&amp;B101,J:J)</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="J101" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="K101" s="5"/>
@@ -6665,11 +6665,11 @@
         <v>1</v>
       </c>
       <c r="I102" s="5">
-        <f>SUMIF($C:$C,"="&amp;B102,J:J)</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="J102" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="K102" s="5"/>
@@ -6709,11 +6709,11 @@
         <v>1</v>
       </c>
       <c r="I103" s="5">
-        <f>SUMIF($C:$C,"="&amp;B103,J:J)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="J103" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="K103" s="5"/>
@@ -6761,11 +6761,11 @@
         <v>1</v>
       </c>
       <c r="I104" s="5">
-        <f>SUMIF($C:$C,"="&amp;B104,J:J)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="J104" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="K104" s="5"/>
@@ -6813,11 +6813,11 @@
         <v>1</v>
       </c>
       <c r="I105" s="5">
-        <f>SUMIF($C:$C,"="&amp;B105,J:J)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="J105" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="K105" s="5"/>
@@ -6865,11 +6865,11 @@
         <v>1</v>
       </c>
       <c r="I106" s="5">
-        <f>SUMIF($C:$C,"="&amp;B106,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J106" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K106" s="5"/>
@@ -6917,11 +6917,11 @@
         <v>1</v>
       </c>
       <c r="I107" s="5">
-        <f>SUMIF($C:$C,"="&amp;B107,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J107" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K107" s="5"/>
@@ -6969,11 +6969,11 @@
         <v>1</v>
       </c>
       <c r="I108" s="5">
-        <f>SUMIF($C:$C,"="&amp;B108,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J108" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K108" s="5" t="s">
@@ -7015,11 +7015,11 @@
         <v>1</v>
       </c>
       <c r="I109" s="5">
-        <f>SUMIF($C:$C,"="&amp;B109,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J109" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K109" s="5" t="s">
@@ -7061,11 +7061,11 @@
         <v>1</v>
       </c>
       <c r="I110" s="5">
-        <f>SUMIF($C:$C,"="&amp;B110,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J110" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K110" s="5" t="s">
@@ -7107,11 +7107,11 @@
         <v>1</v>
       </c>
       <c r="I111" s="5">
-        <f>SUMIF($C:$C,"="&amp;B111,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J111" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K111" s="5" t="s">
@@ -7154,11 +7154,11 @@
         <v>1</v>
       </c>
       <c r="I112" s="5">
-        <f>SUMIF($C:$C,"="&amp;B112,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J112" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K112" s="5"/>
@@ -7192,7 +7192,7 @@
         <v>41</v>
       </c>
       <c r="C113" s="6" t="str">
-        <f t="shared" ref="C113:C176" si="5">F113</f>
+        <f t="shared" ref="C113:C176" si="8">F113</f>
         <v>右足駆動回路v2</v>
       </c>
       <c r="F113" s="1" t="s">
@@ -7203,11 +7203,11 @@
         <v>1</v>
       </c>
       <c r="I113" s="5">
-        <f>SUMIF($C:$C,"="&amp;B113,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J113" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K113" s="3"/>
@@ -7241,7 +7241,7 @@
         <v>41</v>
       </c>
       <c r="C114" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>左足駆動回路v2</v>
       </c>
       <c r="F114" s="1" t="s">
@@ -7252,11 +7252,11 @@
         <v>1</v>
       </c>
       <c r="I114" s="5">
-        <f>SUMIF($C:$C,"="&amp;B114,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J114" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K114" s="3"/>
@@ -7290,7 +7290,7 @@
         <v>41</v>
       </c>
       <c r="C115" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>電子回路ユニット</v>
       </c>
       <c r="F115" s="1" t="s">
@@ -7301,11 +7301,11 @@
         <v>1</v>
       </c>
       <c r="I115" s="5">
-        <f>SUMIF($C:$C,"="&amp;B115,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J115" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K115" s="3" t="s">
@@ -7333,7 +7333,7 @@
         <v>287</v>
       </c>
       <c r="C116" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>腕駆動回路v2</v>
       </c>
       <c r="D116" s="6"/>
@@ -7348,11 +7348,11 @@
         <v>1</v>
       </c>
       <c r="I116" s="5">
-        <f>SUMIF($C:$C,"="&amp;B116,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J116" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K116" s="5"/>
@@ -7386,7 +7386,7 @@
         <v>31</v>
       </c>
       <c r="C117" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>F3-2100</v>
       </c>
       <c r="D117" s="5" t="s">
@@ -7403,11 +7403,11 @@
         <v>2</v>
       </c>
       <c r="I117" s="5">
-        <f>SUMIF($C:$C,"="&amp;B117,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J117" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="K117" s="5"/>
@@ -7435,7 +7435,7 @@
         <v>31</v>
       </c>
       <c r="C118" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>MBIS2-3-2</v>
       </c>
       <c r="D118" s="5"/>
@@ -7452,11 +7452,11 @@
         <v>2</v>
       </c>
       <c r="I118" s="5">
-        <f>SUMIF($C:$C,"="&amp;B118,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J118" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="K118" s="5"/>
@@ -7488,7 +7488,7 @@
         <v>31</v>
       </c>
       <c r="C119" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>CBSTBR2-5</v>
       </c>
       <c r="D119" s="5"/>
@@ -7505,11 +7505,11 @@
         <v>2</v>
       </c>
       <c r="I119" s="5">
-        <f>SUMIF($C:$C,"="&amp;B119,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J119" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="K119" s="5"/>
@@ -7541,7 +7541,7 @@
         <v>31</v>
       </c>
       <c r="C120" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>CBSTBR3-10</v>
       </c>
       <c r="D120" s="5"/>
@@ -7558,11 +7558,11 @@
         <v>5</v>
       </c>
       <c r="I120" s="5">
-        <f>SUMIF($C:$C,"="&amp;B120,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J120" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="K120" s="5"/>
@@ -7594,7 +7594,7 @@
         <v>41</v>
       </c>
       <c r="C121" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>BRL-2011SBE</v>
       </c>
       <c r="D121" s="3" t="s">
@@ -7613,11 +7613,11 @@
         <v>4</v>
       </c>
       <c r="I121" s="5">
-        <f>SUMIF($C:$C,"="&amp;B121,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J121" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="K121" s="3"/>
@@ -7653,7 +7653,7 @@
         <v>41</v>
       </c>
       <c r="C122" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>BRL-311SBE</v>
       </c>
       <c r="D122" s="3" t="s">
@@ -7672,11 +7672,11 @@
         <v>1</v>
       </c>
       <c r="I122" s="5">
-        <f>SUMIF($C:$C,"="&amp;B122,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J122" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K122" s="3"/>
@@ -7712,7 +7712,7 @@
         <v>41</v>
       </c>
       <c r="C123" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>VUY10-55</v>
       </c>
       <c r="E123" s="3" t="s">
@@ -7728,11 +7728,11 @@
         <v>2</v>
       </c>
       <c r="I123" s="5">
-        <f>SUMIF($C:$C,"="&amp;B123,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J123" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="K123" s="3"/>
@@ -7764,7 +7764,7 @@
         <v>41</v>
       </c>
       <c r="C124" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>VUR16-55</v>
       </c>
       <c r="E124" s="3" t="s">
@@ -7780,11 +7780,11 @@
         <v>2</v>
       </c>
       <c r="I124" s="5">
-        <f>SUMIF($C:$C,"="&amp;B124,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J124" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="K124" s="3"/>
@@ -7816,7 +7816,7 @@
         <v>41</v>
       </c>
       <c r="C125" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>小型ファン</v>
       </c>
       <c r="D125" s="3" t="s">
@@ -7835,11 +7835,11 @@
         <v>1</v>
       </c>
       <c r="I125" s="5">
-        <f>SUMIF($C:$C,"="&amp;B125,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J125" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K125" s="3"/>
@@ -7875,7 +7875,7 @@
         <v>41</v>
       </c>
       <c r="C126" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>CFS0.4</v>
       </c>
       <c r="E126" s="3" t="s">
@@ -7889,11 +7889,11 @@
         <v>1</v>
       </c>
       <c r="I126" s="5">
-        <f>SUMIF($C:$C,"="&amp;B126,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J126" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K126" s="3"/>
@@ -7925,7 +7925,7 @@
         <v>41</v>
       </c>
       <c r="C127" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>CBSTBR3-6</v>
       </c>
       <c r="E127" s="3" t="s">
@@ -7941,11 +7941,11 @@
         <v>6</v>
       </c>
       <c r="I127" s="5">
-        <f>SUMIF($C:$C,"="&amp;B127,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J127" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="K127" s="3"/>
@@ -7977,7 +7977,7 @@
         <v>41</v>
       </c>
       <c r="C128" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>CBSTBR2-5</v>
       </c>
       <c r="E128" s="3" t="s">
@@ -7993,11 +7993,11 @@
         <v>8</v>
       </c>
       <c r="I128" s="5">
-        <f>SUMIF($C:$C,"="&amp;B128,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J128" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="K128" s="3"/>
@@ -8029,7 +8029,7 @@
         <v>41</v>
       </c>
       <c r="C129" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>CBSTBR3-10</v>
       </c>
       <c r="E129" s="3" t="s">
@@ -8045,11 +8045,11 @@
         <v>2</v>
       </c>
       <c r="I129" s="5">
-        <f>SUMIF($C:$C,"="&amp;B129,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J129" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="K129" s="3"/>
@@ -8081,7 +8081,7 @@
         <v>41</v>
       </c>
       <c r="C130" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>CBSTSR4-8</v>
       </c>
       <c r="E130" s="3" t="s">
@@ -8097,11 +8097,11 @@
         <v>2</v>
       </c>
       <c r="I130" s="5">
-        <f>SUMIF($C:$C,"="&amp;B130,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J130" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="K130" s="3"/>
@@ -8133,7 +8133,7 @@
         <v>43</v>
       </c>
       <c r="C131" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>DP-C3X20</v>
       </c>
       <c r="D131" s="6" t="s">
@@ -8152,11 +8152,11 @@
         <v>6</v>
       </c>
       <c r="I131" s="5">
-        <f>SUMIF($C:$C,"="&amp;B131,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J131" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="K131" s="5" t="s">
@@ -8180,7 +8180,7 @@
         <v>43</v>
       </c>
       <c r="C132" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>SS_10GL13</v>
       </c>
       <c r="D132" s="6" t="s">
@@ -8199,11 +8199,11 @@
         <v>2</v>
       </c>
       <c r="I132" s="5">
-        <f>SUMIF($C:$C,"="&amp;B132,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J132" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="K132" s="5"/>
@@ -8229,7 +8229,7 @@
         <v>43</v>
       </c>
       <c r="C133" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>PJLS10-5</v>
       </c>
       <c r="D133" s="6" t="s">
@@ -8248,11 +8248,11 @@
         <v>2</v>
       </c>
       <c r="I133" s="5">
-        <f>SUMIF($C:$C,"="&amp;B133,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J133" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="K133" s="5" t="s">
@@ -8284,7 +8284,7 @@
         <v>43</v>
       </c>
       <c r="C134" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>CLJW6-8-12.0</v>
       </c>
       <c r="D134" s="6"/>
@@ -8301,11 +8301,11 @@
         <v>2</v>
       </c>
       <c r="I134" s="5">
-        <f>SUMIF($C:$C,"="&amp;B134,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J134" s="5">
-        <f t="shared" ref="J134:J197" si="6">H134*I134</f>
+        <f t="shared" ref="J134:J197" si="9">H134*I134</f>
         <v>2</v>
       </c>
       <c r="K134" s="5"/>
@@ -8335,7 +8335,7 @@
         <v>43</v>
       </c>
       <c r="C135" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>YDH3007C05F</v>
       </c>
       <c r="D135" s="6" t="s">
@@ -8352,11 +8352,11 @@
         <v>1</v>
       </c>
       <c r="I135" s="5">
-        <f>SUMIF($C:$C,"="&amp;B135,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J135" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K135" s="5"/>
@@ -8386,7 +8386,7 @@
         <v>43</v>
       </c>
       <c r="C136" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>FWSJW-D8-V6-T6.0</v>
       </c>
       <c r="D136" s="6"/>
@@ -8403,11 +8403,11 @@
         <v>2</v>
       </c>
       <c r="I136" s="5">
-        <f>SUMIF($C:$C,"="&amp;B136,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J136" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="K136" s="5"/>
@@ -8437,7 +8437,7 @@
         <v>43</v>
       </c>
       <c r="C137" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>B6805ZZ</v>
       </c>
       <c r="D137" s="6"/>
@@ -8454,11 +8454,11 @@
         <v>3</v>
       </c>
       <c r="I137" s="5">
-        <f>SUMIF($C:$C,"="&amp;B137,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J137" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="K137" s="5"/>
@@ -8488,7 +8488,7 @@
         <v>43</v>
       </c>
       <c r="C138" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>CBSTBR3-10</v>
       </c>
       <c r="D138" s="6"/>
@@ -8505,11 +8505,11 @@
         <v>4</v>
       </c>
       <c r="I138" s="5">
-        <f>SUMIF($C:$C,"="&amp;B138,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J138" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="K138" s="5"/>
@@ -8539,7 +8539,7 @@
         <v>43</v>
       </c>
       <c r="C139" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>CBSTBR3-6</v>
       </c>
       <c r="D139" s="6"/>
@@ -8556,11 +8556,11 @@
         <v>10</v>
       </c>
       <c r="I139" s="5">
-        <f>SUMIF($C:$C,"="&amp;B139,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J139" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="K139" s="5"/>
@@ -8590,7 +8590,7 @@
         <v>43</v>
       </c>
       <c r="C140" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>CBSTBR2-10</v>
       </c>
       <c r="D140" s="6"/>
@@ -8607,11 +8607,11 @@
         <v>4</v>
       </c>
       <c r="I140" s="5">
-        <f>SUMIF($C:$C,"="&amp;B140,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J140" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="K140" s="5"/>
@@ -8641,7 +8641,7 @@
         <v>43</v>
       </c>
       <c r="C141" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>SFHRW6-103.0-M3-N3</v>
       </c>
       <c r="D141" s="6"/>
@@ -8654,11 +8654,11 @@
         <v>2</v>
       </c>
       <c r="I141" s="5">
-        <f>SUMIF($C:$C,"="&amp;B141,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J141" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="K141" s="5"/>
@@ -8684,7 +8684,7 @@
         <v>43</v>
       </c>
       <c r="C142" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>SFRHH6-109.0-F2.5-P5-T2.5-M3</v>
       </c>
       <c r="D142" s="6"/>
@@ -8697,11 +8697,11 @@
         <v>2</v>
       </c>
       <c r="I142" s="5">
-        <f>SUMIF($C:$C,"="&amp;B142,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J142" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="K142" s="5"/>
@@ -8727,7 +8727,7 @@
         <v>43</v>
       </c>
       <c r="C143" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>SFRMGH8-15.0-F2.8-P6-T4.9-M3</v>
       </c>
       <c r="D143" s="6"/>
@@ -8742,11 +8742,11 @@
         <v>6</v>
       </c>
       <c r="I143" s="5">
-        <f>SUMIF($C:$C,"="&amp;B143,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J143" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="K143" s="5"/>
@@ -8776,7 +8776,7 @@
         <v>89</v>
       </c>
       <c r="C144" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>ARL-360BE</v>
       </c>
       <c r="D144" s="6" t="s">
@@ -8795,11 +8795,11 @@
         <v>2</v>
       </c>
       <c r="I144" s="5">
-        <f>SUMIF($C:$C,"="&amp;B144,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J144" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="K144" s="5"/>
@@ -8835,7 +8835,7 @@
         <v>89</v>
       </c>
       <c r="C145" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>WSJK8-3-2</v>
       </c>
       <c r="D145" s="6"/>
@@ -8852,11 +8852,11 @@
         <v>2</v>
       </c>
       <c r="I145" s="5">
-        <f>SUMIF($C:$C,"="&amp;B145,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J145" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="K145" s="5"/>
@@ -8888,7 +8888,7 @@
         <v>89</v>
       </c>
       <c r="C146" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>CBSTBR3-10</v>
       </c>
       <c r="D146" s="6"/>
@@ -8905,11 +8905,11 @@
         <v>2</v>
       </c>
       <c r="I146" s="5">
-        <f>SUMIF($C:$C,"="&amp;B146,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J146" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="K146" s="5"/>
@@ -8941,7 +8941,7 @@
         <v>89</v>
       </c>
       <c r="C147" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>CBSTBR3-6</v>
       </c>
       <c r="D147" s="6"/>
@@ -8958,11 +8958,11 @@
         <v>2</v>
       </c>
       <c r="I147" s="5">
-        <f>SUMIF($C:$C,"="&amp;B147,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J147" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="K147" s="5"/>
@@ -8994,7 +8994,7 @@
         <v>89</v>
       </c>
       <c r="C148" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>MPBZ6-15</v>
       </c>
       <c r="D148" s="6"/>
@@ -9011,11 +9011,11 @@
         <v>2</v>
       </c>
       <c r="I148" s="5">
-        <f>SUMIF($C:$C,"="&amp;B148,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J148" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="K148" s="5"/>
@@ -9047,7 +9047,7 @@
         <v>147</v>
       </c>
       <c r="C149" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>ABETTF6-75.0-M3-N3</v>
       </c>
       <c r="D149" s="6" t="s">
@@ -9066,11 +9066,11 @@
         <v>2</v>
       </c>
       <c r="I149" s="5">
-        <f>SUMIF($C:$C,"="&amp;B149,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J149" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="K149" s="5"/>
@@ -9102,7 +9102,7 @@
         <v>147</v>
       </c>
       <c r="C150" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>CBSTBR3-10</v>
       </c>
       <c r="D150" s="6"/>
@@ -9119,11 +9119,11 @@
         <v>4</v>
       </c>
       <c r="I150" s="5">
-        <f>SUMIF($C:$C,"="&amp;B150,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J150" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="K150" s="5"/>
@@ -9155,7 +9155,7 @@
         <v>147</v>
       </c>
       <c r="C151" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>BFLB6-5</v>
       </c>
       <c r="D151" s="6"/>
@@ -9172,11 +9172,11 @@
         <v>4</v>
       </c>
       <c r="I151" s="5">
-        <f>SUMIF($C:$C,"="&amp;B151,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J151" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="K151" s="5"/>
@@ -9208,7 +9208,7 @@
         <v>165</v>
       </c>
       <c r="C152" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>DPS-C6X20</v>
       </c>
       <c r="D152" s="6" t="s">
@@ -9227,11 +9227,11 @@
         <v>2</v>
       </c>
       <c r="I152" s="5">
-        <f>SUMIF($C:$C,"="&amp;B152,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J152" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="K152" s="5"/>
@@ -9267,7 +9267,7 @@
         <v>155</v>
       </c>
       <c r="C153" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>ABETTF6-90.0-M3-N3</v>
       </c>
       <c r="D153" s="6"/>
@@ -9284,11 +9284,11 @@
         <v>5</v>
       </c>
       <c r="I153" s="5">
-        <f>SUMIF($C:$C,"="&amp;B153,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J153" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="K153" s="5"/>
@@ -9320,7 +9320,7 @@
         <v>155</v>
       </c>
       <c r="C154" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>BFLB6-5</v>
       </c>
       <c r="D154" s="6"/>
@@ -9337,11 +9337,11 @@
         <v>2</v>
       </c>
       <c r="I154" s="5">
-        <f>SUMIF($C:$C,"="&amp;B154,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J154" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="K154" s="5"/>
@@ -9373,7 +9373,7 @@
         <v>155</v>
       </c>
       <c r="C155" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>CBSTBR3-10</v>
       </c>
       <c r="D155" s="6"/>
@@ -9390,11 +9390,11 @@
         <v>10</v>
       </c>
       <c r="I155" s="5">
-        <f>SUMIF($C:$C,"="&amp;B155,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J155" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="K155" s="5"/>
@@ -9426,7 +9426,7 @@
         <v>155</v>
       </c>
       <c r="C156" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>CBSTSR4-8</v>
       </c>
       <c r="D156" s="6"/>
@@ -9443,11 +9443,11 @@
         <v>4</v>
       </c>
       <c r="I156" s="5">
-        <f>SUMIF($C:$C,"="&amp;B156,J:J)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J156" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="K156" s="5"/>
@@ -9479,7 +9479,7 @@
         <v>168</v>
       </c>
       <c r="C157" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>CL-306E</v>
       </c>
       <c r="D157" s="6" t="s">
@@ -9498,11 +9498,11 @@
         <v>1</v>
       </c>
       <c r="I157" s="5">
-        <f>SUMIF($C:$C,"="&amp;B157,J:J)</f>
+        <f t="shared" ref="I157:I220" si="10">SUMIF($C:$C,"="&amp;B157,J:J)</f>
         <v>1</v>
       </c>
       <c r="J157" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K157" s="5"/>
@@ -9538,7 +9538,7 @@
         <v>168</v>
       </c>
       <c r="C158" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>CBSTBR3-10</v>
       </c>
       <c r="D158" s="6"/>
@@ -9555,11 +9555,11 @@
         <v>1</v>
       </c>
       <c r="I158" s="5">
-        <f>SUMIF($C:$C,"="&amp;B158,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J158" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K158" s="5"/>
@@ -9591,7 +9591,7 @@
         <v>172</v>
       </c>
       <c r="C159" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>CL-306E</v>
       </c>
       <c r="D159" s="6" t="s">
@@ -9610,11 +9610,11 @@
         <v>1</v>
       </c>
       <c r="I159" s="5">
-        <f>SUMIF($C:$C,"="&amp;B159,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J159" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K159" s="5"/>
@@ -9650,7 +9650,7 @@
         <v>172</v>
       </c>
       <c r="C160" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>CBSTBR3-10</v>
       </c>
       <c r="D160" s="6"/>
@@ -9667,11 +9667,11 @@
         <v>1</v>
       </c>
       <c r="I160" s="5">
-        <f>SUMIF($C:$C,"="&amp;B160,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J160" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K160" s="5"/>
@@ -9703,7 +9703,7 @@
         <v>214</v>
       </c>
       <c r="C161" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>ARL-340BE</v>
       </c>
       <c r="D161" s="6" t="s">
@@ -9722,11 +9722,11 @@
         <v>7</v>
       </c>
       <c r="I161" s="5">
-        <f>SUMIF($C:$C,"="&amp;B161,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J161" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="K161" s="5"/>
@@ -9762,7 +9762,7 @@
         <v>214</v>
       </c>
       <c r="C162" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>HTBN474S3M-60</v>
       </c>
       <c r="D162" s="6" t="s">
@@ -9781,11 +9781,11 @@
         <v>1</v>
       </c>
       <c r="I162" s="5">
-        <f>SUMIF($C:$C,"="&amp;B162,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J162" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K162" s="5"/>
@@ -9821,7 +9821,7 @@
         <v>214</v>
       </c>
       <c r="C163" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>CBSTBR3-6</v>
       </c>
       <c r="D163" s="6"/>
@@ -9838,11 +9838,11 @@
         <v>28</v>
       </c>
       <c r="I163" s="5">
-        <f>SUMIF($C:$C,"="&amp;B163,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J163" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>28</v>
       </c>
       <c r="K163" s="5"/>
@@ -9874,7 +9874,7 @@
         <v>214</v>
       </c>
       <c r="C164" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>CBSTBR3-10</v>
       </c>
       <c r="D164" s="6"/>
@@ -9891,11 +9891,11 @@
         <v>1</v>
       </c>
       <c r="I164" s="5">
-        <f>SUMIF($C:$C,"="&amp;B164,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J164" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K164" s="5"/>
@@ -9927,7 +9927,7 @@
         <v>214</v>
       </c>
       <c r="C165" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>MPFZ10-8</v>
       </c>
       <c r="D165" s="6"/>
@@ -9944,11 +9944,11 @@
         <v>2</v>
       </c>
       <c r="I165" s="5">
-        <f>SUMIF($C:$C,"="&amp;B165,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J165" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="K165" s="5"/>
@@ -9980,7 +9980,7 @@
         <v>214</v>
       </c>
       <c r="C166" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>CB2.6-5</v>
       </c>
       <c r="D166" s="6"/>
@@ -9997,11 +9997,11 @@
         <v>4</v>
       </c>
       <c r="I166" s="5">
-        <f>SUMIF($C:$C,"="&amp;B166,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J166" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="K166" s="5"/>
@@ -10033,7 +10033,7 @@
         <v>214</v>
       </c>
       <c r="C167" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>RS380-PH</v>
       </c>
       <c r="D167" s="6" t="s">
@@ -10052,11 +10052,11 @@
         <v>2</v>
       </c>
       <c r="I167" s="5">
-        <f>SUMIF($C:$C,"="&amp;B167,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J167" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="K167" s="5" t="s">
@@ -10086,7 +10086,7 @@
         <v>214</v>
       </c>
       <c r="C168" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>SS0.5-10</v>
       </c>
       <c r="D168" s="6" t="s">
@@ -10105,11 +10105,11 @@
         <v>2</v>
       </c>
       <c r="I168" s="5">
-        <f>SUMIF($C:$C,"="&amp;B168,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J168" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="K168" s="5"/>
@@ -10147,7 +10147,7 @@
         <v>214</v>
       </c>
       <c r="C169" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>CLJW6-8-40.0</v>
       </c>
       <c r="D169" s="6"/>
@@ -10164,11 +10164,11 @@
         <v>4</v>
       </c>
       <c r="I169" s="5">
-        <f>SUMIF($C:$C,"="&amp;B169,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J169" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="K169" s="5"/>
@@ -10200,7 +10200,7 @@
         <v>214</v>
       </c>
       <c r="C170" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>CLJW6-8-38.0</v>
       </c>
       <c r="D170" s="6"/>
@@ -10217,11 +10217,11 @@
         <v>4</v>
       </c>
       <c r="I170" s="5">
-        <f>SUMIF($C:$C,"="&amp;B170,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J170" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="K170" s="5"/>
@@ -10253,7 +10253,7 @@
         <v>209</v>
       </c>
       <c r="C171" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>ARL-340BE</v>
       </c>
       <c r="D171" s="6"/>
@@ -10268,11 +10268,11 @@
         <v>1</v>
       </c>
       <c r="I171" s="5">
-        <f>SUMIF($C:$C,"="&amp;B171,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J171" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K171" s="5"/>
@@ -10308,7 +10308,7 @@
         <v>209</v>
       </c>
       <c r="C172" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>CLJW6-8-15.5</v>
       </c>
       <c r="D172" s="6"/>
@@ -10325,11 +10325,11 @@
         <v>1</v>
       </c>
       <c r="I172" s="5">
-        <f>SUMIF($C:$C,"="&amp;B172,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J172" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K172" s="5"/>
@@ -10361,7 +10361,7 @@
         <v>209</v>
       </c>
       <c r="C173" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>FWSJW-D8-V6-T6.0</v>
       </c>
       <c r="D173" s="6"/>
@@ -10378,11 +10378,11 @@
         <v>2</v>
       </c>
       <c r="I173" s="5">
-        <f>SUMIF($C:$C,"="&amp;B173,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J173" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="K173" s="5"/>
@@ -10414,7 +10414,7 @@
         <v>209</v>
       </c>
       <c r="C174" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>FWSJW-D8-V6-T5.5</v>
       </c>
       <c r="D174" s="6"/>
@@ -10431,11 +10431,11 @@
         <v>1</v>
       </c>
       <c r="I174" s="5">
-        <f>SUMIF($C:$C,"="&amp;B174,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J174" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K174" s="5"/>
@@ -10467,7 +10467,7 @@
         <v>209</v>
       </c>
       <c r="C175" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>FL678ZZ</v>
       </c>
       <c r="D175" s="6"/>
@@ -10484,11 +10484,11 @@
         <v>2</v>
       </c>
       <c r="I175" s="5">
-        <f>SUMIF($C:$C,"="&amp;B175,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J175" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="K175" s="5"/>
@@ -10520,7 +10520,7 @@
         <v>209</v>
       </c>
       <c r="C176" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>SFB3-10</v>
       </c>
       <c r="D176" s="6" t="s">
@@ -10539,11 +10539,11 @@
         <v>9</v>
       </c>
       <c r="I176" s="5">
-        <f>SUMIF($C:$C,"="&amp;B176,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J176" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="K176" s="5"/>
@@ -10571,7 +10571,7 @@
         <v>209</v>
       </c>
       <c r="C177" s="6" t="str">
-        <f t="shared" ref="C177:C239" si="7">F177</f>
+        <f t="shared" ref="C177:C239" si="11">F177</f>
         <v>CBSTBR3-10</v>
       </c>
       <c r="D177" s="6"/>
@@ -10588,11 +10588,11 @@
         <v>3</v>
       </c>
       <c r="I177" s="5">
-        <f>SUMIF($C:$C,"="&amp;B177,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J177" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="K177" s="5"/>
@@ -10624,7 +10624,7 @@
         <v>248</v>
       </c>
       <c r="C178" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>ARL-340BE</v>
       </c>
       <c r="D178" s="6"/>
@@ -10639,11 +10639,11 @@
         <v>1</v>
       </c>
       <c r="I178" s="5">
-        <f>SUMIF($C:$C,"="&amp;B178,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J178" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K178" s="5"/>
@@ -10679,7 +10679,7 @@
         <v>248</v>
       </c>
       <c r="C179" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>CLJW6-8-15.5</v>
       </c>
       <c r="D179" s="6"/>
@@ -10696,11 +10696,11 @@
         <v>1</v>
       </c>
       <c r="I179" s="5">
-        <f>SUMIF($C:$C,"="&amp;B179,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J179" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K179" s="5"/>
@@ -10732,7 +10732,7 @@
         <v>248</v>
       </c>
       <c r="C180" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>FWSJW-D8-V6-T6.0</v>
       </c>
       <c r="D180" s="6"/>
@@ -10749,11 +10749,11 @@
         <v>2</v>
       </c>
       <c r="I180" s="5">
-        <f>SUMIF($C:$C,"="&amp;B180,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J180" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="K180" s="5"/>
@@ -10785,7 +10785,7 @@
         <v>248</v>
       </c>
       <c r="C181" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>FWSJW-D8-V6-T5.5</v>
       </c>
       <c r="D181" s="6"/>
@@ -10802,11 +10802,11 @@
         <v>1</v>
       </c>
       <c r="I181" s="5">
-        <f>SUMIF($C:$C,"="&amp;B181,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J181" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K181" s="5"/>
@@ -10838,7 +10838,7 @@
         <v>248</v>
       </c>
       <c r="C182" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>FL678ZZ</v>
       </c>
       <c r="D182" s="6"/>
@@ -10855,11 +10855,11 @@
         <v>2</v>
       </c>
       <c r="I182" s="5">
-        <f>SUMIF($C:$C,"="&amp;B182,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J182" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="K182" s="5"/>
@@ -10891,7 +10891,7 @@
         <v>248</v>
       </c>
       <c r="C183" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>SFB3-10</v>
       </c>
       <c r="D183" s="6" t="s">
@@ -10910,11 +10910,11 @@
         <v>9</v>
       </c>
       <c r="I183" s="5">
-        <f>SUMIF($C:$C,"="&amp;B183,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J183" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="K183" s="5"/>
@@ -10942,7 +10942,7 @@
         <v>248</v>
       </c>
       <c r="C184" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>CBSTBR3-10</v>
       </c>
       <c r="D184" s="6"/>
@@ -10959,11 +10959,11 @@
         <v>3</v>
       </c>
       <c r="I184" s="5">
-        <f>SUMIF($C:$C,"="&amp;B184,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J184" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="K184" s="5"/>
@@ -10995,7 +10995,7 @@
         <v>249</v>
       </c>
       <c r="C185" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>B6700ZZ</v>
       </c>
       <c r="D185" s="6"/>
@@ -11012,11 +11012,11 @@
         <v>1</v>
       </c>
       <c r="I185" s="5">
-        <f>SUMIF($C:$C,"="&amp;B185,J:J)</f>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="J185" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="K185" s="5"/>
@@ -11048,7 +11048,7 @@
         <v>249</v>
       </c>
       <c r="C186" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>SFB3-5</v>
       </c>
       <c r="D186" s="6" t="s">
@@ -11067,11 +11067,11 @@
         <v>2</v>
       </c>
       <c r="I186" s="5">
-        <f>SUMIF($C:$C,"="&amp;B186,J:J)</f>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="J186" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="K186" s="5"/>
@@ -11099,7 +11099,7 @@
         <v>249</v>
       </c>
       <c r="C187" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>CBSTBR3-4</v>
       </c>
       <c r="D187" s="6"/>
@@ -11116,11 +11116,11 @@
         <v>3</v>
       </c>
       <c r="I187" s="5">
-        <f>SUMIF($C:$C,"="&amp;B187,J:J)</f>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="J187" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>18</v>
       </c>
       <c r="K187" s="5"/>
@@ -11152,7 +11152,7 @@
         <v>249</v>
       </c>
       <c r="C188" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>WSSB5-3-2</v>
       </c>
       <c r="D188" s="6"/>
@@ -11169,11 +11169,11 @@
         <v>1</v>
       </c>
       <c r="I188" s="5">
-        <f>SUMIF($C:$C,"="&amp;B188,J:J)</f>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="J188" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="K188" s="5"/>
@@ -11205,7 +11205,7 @@
         <v>259</v>
       </c>
       <c r="C189" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>ARL-340BE</v>
       </c>
       <c r="D189" s="6" t="s">
@@ -11224,11 +11224,11 @@
         <v>7</v>
       </c>
       <c r="I189" s="5">
-        <f>SUMIF($C:$C,"="&amp;B189,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J189" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="K189" s="5"/>
@@ -11264,7 +11264,7 @@
         <v>259</v>
       </c>
       <c r="C190" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>HTBN474S3M-60</v>
       </c>
       <c r="D190" s="6" t="s">
@@ -11283,11 +11283,11 @@
         <v>1</v>
       </c>
       <c r="I190" s="5">
-        <f>SUMIF($C:$C,"="&amp;B190,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J190" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K190" s="5"/>
@@ -11323,7 +11323,7 @@
         <v>259</v>
       </c>
       <c r="C191" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>CBSTBR3-6</v>
       </c>
       <c r="D191" s="6"/>
@@ -11340,11 +11340,11 @@
         <v>28</v>
       </c>
       <c r="I191" s="5">
-        <f>SUMIF($C:$C,"="&amp;B191,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J191" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>28</v>
       </c>
       <c r="K191" s="5"/>
@@ -11376,7 +11376,7 @@
         <v>259</v>
       </c>
       <c r="C192" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>CBSTBR3-10</v>
       </c>
       <c r="D192" s="6"/>
@@ -11393,11 +11393,11 @@
         <v>1</v>
       </c>
       <c r="I192" s="5">
-        <f>SUMIF($C:$C,"="&amp;B192,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J192" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K192" s="5"/>
@@ -11429,7 +11429,7 @@
         <v>259</v>
       </c>
       <c r="C193" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>MPFZ10-8</v>
       </c>
       <c r="D193" s="6"/>
@@ -11446,11 +11446,11 @@
         <v>2</v>
       </c>
       <c r="I193" s="5">
-        <f>SUMIF($C:$C,"="&amp;B193,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J193" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="K193" s="5"/>
@@ -11482,7 +11482,7 @@
         <v>259</v>
       </c>
       <c r="C194" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>CB2.6-5</v>
       </c>
       <c r="D194" s="6"/>
@@ -11499,11 +11499,11 @@
         <v>4</v>
       </c>
       <c r="I194" s="5">
-        <f>SUMIF($C:$C,"="&amp;B194,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J194" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="K194" s="5"/>
@@ -11535,7 +11535,7 @@
         <v>259</v>
       </c>
       <c r="C195" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>CLJW6-8-40.0</v>
       </c>
       <c r="D195" s="6"/>
@@ -11552,11 +11552,11 @@
         <v>4</v>
       </c>
       <c r="I195" s="5">
-        <f>SUMIF($C:$C,"="&amp;B195,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J195" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="K195" s="5"/>
@@ -11588,7 +11588,7 @@
         <v>259</v>
       </c>
       <c r="C196" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>CLJW6-8-38.0</v>
       </c>
       <c r="D196" s="6"/>
@@ -11605,11 +11605,11 @@
         <v>4</v>
       </c>
       <c r="I196" s="5">
-        <f>SUMIF($C:$C,"="&amp;B196,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J196" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="K196" s="5"/>
@@ -11641,7 +11641,7 @@
         <v>259</v>
       </c>
       <c r="C197" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>RS380-PH</v>
       </c>
       <c r="D197" s="6" t="s">
@@ -11660,11 +11660,11 @@
         <v>2</v>
       </c>
       <c r="I197" s="5">
-        <f>SUMIF($C:$C,"="&amp;B197,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J197" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="K197" s="5" t="s">
@@ -11694,7 +11694,7 @@
         <v>259</v>
       </c>
       <c r="C198" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>SS0.5-10</v>
       </c>
       <c r="D198" s="6" t="s">
@@ -11713,11 +11713,11 @@
         <v>2</v>
       </c>
       <c r="I198" s="5">
-        <f>SUMIF($C:$C,"="&amp;B198,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J198" s="5">
-        <f t="shared" ref="J198:J241" si="8">H198*I198</f>
+        <f t="shared" ref="J198:J241" si="12">H198*I198</f>
         <v>2</v>
       </c>
       <c r="K198" s="5"/>
@@ -11755,7 +11755,7 @@
         <v>263</v>
       </c>
       <c r="C199" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>ARL-340BE</v>
       </c>
       <c r="D199" s="6"/>
@@ -11770,11 +11770,11 @@
         <v>1</v>
       </c>
       <c r="I199" s="5">
-        <f>SUMIF($C:$C,"="&amp;B199,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J199" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="K199" s="5"/>
@@ -11808,7 +11808,7 @@
         <v>263</v>
       </c>
       <c r="C200" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>CLJW6-8-15.5</v>
       </c>
       <c r="D200" s="6"/>
@@ -11825,11 +11825,11 @@
         <v>1</v>
       </c>
       <c r="I200" s="5">
-        <f>SUMIF($C:$C,"="&amp;B200,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J200" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="K200" s="5"/>
@@ -11861,7 +11861,7 @@
         <v>263</v>
       </c>
       <c r="C201" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>FWSJW-D8-V6-T6.0</v>
       </c>
       <c r="D201" s="6"/>
@@ -11878,11 +11878,11 @@
         <v>2</v>
       </c>
       <c r="I201" s="5">
-        <f>SUMIF($C:$C,"="&amp;B201,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J201" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="K201" s="5"/>
@@ -11914,7 +11914,7 @@
         <v>263</v>
       </c>
       <c r="C202" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>FWSJW-D8-V6-T5.5</v>
       </c>
       <c r="D202" s="6"/>
@@ -11931,11 +11931,11 @@
         <v>1</v>
       </c>
       <c r="I202" s="5">
-        <f>SUMIF($C:$C,"="&amp;B202,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J202" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="K202" s="5"/>
@@ -11967,7 +11967,7 @@
         <v>263</v>
       </c>
       <c r="C203" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>FL678ZZ</v>
       </c>
       <c r="D203" s="6"/>
@@ -11984,11 +11984,11 @@
         <v>2</v>
       </c>
       <c r="I203" s="5">
-        <f>SUMIF($C:$C,"="&amp;B203,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J203" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="K203" s="5"/>
@@ -12020,7 +12020,7 @@
         <v>263</v>
       </c>
       <c r="C204" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>SFB3-10</v>
       </c>
       <c r="D204" s="6" t="s">
@@ -12039,11 +12039,11 @@
         <v>9</v>
       </c>
       <c r="I204" s="5">
-        <f>SUMIF($C:$C,"="&amp;B204,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J204" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="K204" s="5"/>
@@ -12071,7 +12071,7 @@
         <v>263</v>
       </c>
       <c r="C205" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>CBSTBR3-10</v>
       </c>
       <c r="D205" s="6"/>
@@ -12088,11 +12088,11 @@
         <v>3</v>
       </c>
       <c r="I205" s="5">
-        <f>SUMIF($C:$C,"="&amp;B205,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J205" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="K205" s="5"/>
@@ -12124,7 +12124,7 @@
         <v>264</v>
       </c>
       <c r="C206" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>ARL-340BE</v>
       </c>
       <c r="D206" s="6"/>
@@ -12139,11 +12139,11 @@
         <v>1</v>
       </c>
       <c r="I206" s="5">
-        <f>SUMIF($C:$C,"="&amp;B206,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J206" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="K206" s="5"/>
@@ -12177,7 +12177,7 @@
         <v>264</v>
       </c>
       <c r="C207" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>CLJW6-8-15.5</v>
       </c>
       <c r="D207" s="6"/>
@@ -12194,11 +12194,11 @@
         <v>1</v>
       </c>
       <c r="I207" s="5">
-        <f>SUMIF($C:$C,"="&amp;B207,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J207" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="K207" s="5"/>
@@ -12230,7 +12230,7 @@
         <v>264</v>
       </c>
       <c r="C208" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>FWSJW-D8-V6-T6.0</v>
       </c>
       <c r="D208" s="6"/>
@@ -12247,11 +12247,11 @@
         <v>2</v>
       </c>
       <c r="I208" s="5">
-        <f>SUMIF($C:$C,"="&amp;B208,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J208" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="K208" s="5"/>
@@ -12283,7 +12283,7 @@
         <v>264</v>
       </c>
       <c r="C209" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>FWSJW-D8-V6-T5.5</v>
       </c>
       <c r="D209" s="6"/>
@@ -12300,11 +12300,11 @@
         <v>1</v>
       </c>
       <c r="I209" s="5">
-        <f>SUMIF($C:$C,"="&amp;B209,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J209" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="K209" s="5"/>
@@ -12336,7 +12336,7 @@
         <v>264</v>
       </c>
       <c r="C210" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>FL678ZZ</v>
       </c>
       <c r="D210" s="6"/>
@@ -12353,11 +12353,11 @@
         <v>2</v>
       </c>
       <c r="I210" s="5">
-        <f>SUMIF($C:$C,"="&amp;B210,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J210" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="K210" s="5"/>
@@ -12389,7 +12389,7 @@
         <v>264</v>
       </c>
       <c r="C211" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>SFB3-10</v>
       </c>
       <c r="D211" s="6" t="s">
@@ -12408,11 +12408,11 @@
         <v>9</v>
       </c>
       <c r="I211" s="5">
-        <f>SUMIF($C:$C,"="&amp;B211,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J211" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="K211" s="5"/>
@@ -12440,7 +12440,7 @@
         <v>264</v>
       </c>
       <c r="C212" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>CBSTBR3-10</v>
       </c>
       <c r="D212" s="6"/>
@@ -12457,11 +12457,11 @@
         <v>3</v>
       </c>
       <c r="I212" s="5">
-        <f>SUMIF($C:$C,"="&amp;B212,J:J)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J212" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="K212" s="5"/>
@@ -12493,7 +12493,7 @@
         <v>266</v>
       </c>
       <c r="C213" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>B6700ZZ</v>
       </c>
       <c r="D213" s="6"/>
@@ -12510,11 +12510,11 @@
         <v>1</v>
       </c>
       <c r="I213" s="5">
-        <f>SUMIF($C:$C,"="&amp;B213,J:J)</f>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="J213" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="K213" s="5"/>
@@ -12546,7 +12546,7 @@
         <v>266</v>
       </c>
       <c r="C214" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>SFB3-5</v>
       </c>
       <c r="D214" s="6" t="s">
@@ -12565,11 +12565,11 @@
         <v>2</v>
       </c>
       <c r="I214" s="5">
-        <f>SUMIF($C:$C,"="&amp;B214,J:J)</f>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="J214" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>12</v>
       </c>
       <c r="K214" s="5"/>
@@ -12597,7 +12597,7 @@
         <v>266</v>
       </c>
       <c r="C215" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>CBSTBR3-4</v>
       </c>
       <c r="D215" s="6"/>
@@ -12614,11 +12614,11 @@
         <v>3</v>
       </c>
       <c r="I215" s="5">
-        <f>SUMIF($C:$C,"="&amp;B215,J:J)</f>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="J215" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>18</v>
       </c>
       <c r="K215" s="5"/>
@@ -12650,7 +12650,7 @@
         <v>266</v>
       </c>
       <c r="C216" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>WSSB5-3-2</v>
       </c>
       <c r="D216" s="6"/>
@@ -12667,11 +12667,11 @@
         <v>1</v>
       </c>
       <c r="I216" s="5">
-        <f>SUMIF($C:$C,"="&amp;B216,J:J)</f>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="J216" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="K216" s="5"/>
@@ -12703,7 +12703,7 @@
         <v>207</v>
       </c>
       <c r="C217" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>ARL-340BE</v>
       </c>
       <c r="D217" s="6" t="s">
@@ -12722,11 +12722,11 @@
         <v>1</v>
       </c>
       <c r="I217" s="5">
-        <f>SUMIF($C:$C,"="&amp;B217,J:J)</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="J217" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="K217" s="5"/>
@@ -12762,7 +12762,7 @@
         <v>207</v>
       </c>
       <c r="C218" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>VUR6-20</v>
       </c>
       <c r="D218" s="6"/>
@@ -12779,11 +12779,11 @@
         <v>1</v>
       </c>
       <c r="I218" s="5">
-        <f>SUMIF($C:$C,"="&amp;B218,J:J)</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="J218" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="K218" s="5"/>
@@ -12815,7 +12815,7 @@
         <v>276</v>
       </c>
       <c r="C219" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>CBSTBR3-6</v>
       </c>
       <c r="D219" s="6"/>
@@ -12832,11 +12832,11 @@
         <v>3</v>
       </c>
       <c r="I219" s="5">
-        <f>SUMIF($C:$C,"="&amp;B219,J:J)</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="J219" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="K219" s="5"/>
@@ -12868,7 +12868,7 @@
         <v>207</v>
       </c>
       <c r="C220" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>SCCN6-6</v>
       </c>
       <c r="D220" s="6"/>
@@ -12885,11 +12885,11 @@
         <v>1</v>
       </c>
       <c r="I220" s="5">
-        <f>SUMIF($C:$C,"="&amp;B220,J:J)</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="J220" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="K220" s="5"/>
@@ -12921,7 +12921,7 @@
         <v>207</v>
       </c>
       <c r="C221" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>FWSJW-D8-V6-T5.5</v>
       </c>
       <c r="D221" s="6"/>
@@ -12938,11 +12938,11 @@
         <v>1</v>
       </c>
       <c r="I221" s="5">
-        <f>SUMIF($C:$C,"="&amp;B221,J:J)</f>
+        <f t="shared" ref="I221:I284" si="13">SUMIF($C:$C,"="&amp;B221,J:J)</f>
         <v>2</v>
       </c>
       <c r="J221" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="K221" s="5"/>
@@ -12974,7 +12974,7 @@
         <v>207</v>
       </c>
       <c r="C222" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>MPBRU6-8</v>
       </c>
       <c r="D222" s="6"/>
@@ -12991,11 +12991,11 @@
         <v>1</v>
       </c>
       <c r="I222" s="5">
-        <f>SUMIF($C:$C,"="&amp;B222,J:J)</f>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="J222" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="K222" s="5"/>
@@ -13027,7 +13027,7 @@
         <v>207</v>
       </c>
       <c r="C223" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>WSSB8-6-1.5</v>
       </c>
       <c r="D223" s="6"/>
@@ -13044,11 +13044,11 @@
         <v>1</v>
       </c>
       <c r="I223" s="5">
-        <f>SUMIF($C:$C,"="&amp;B223,J:J)</f>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="J223" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="K223" s="5"/>
@@ -13080,7 +13080,7 @@
         <v>287</v>
       </c>
       <c r="C224" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>ARL-340BE</v>
       </c>
       <c r="D224" s="6" t="s">
@@ -13099,11 +13099,11 @@
         <v>3</v>
       </c>
       <c r="I224" s="5">
-        <f>SUMIF($C:$C,"="&amp;B224,J:J)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="J224" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="K224" s="5"/>
@@ -13139,7 +13139,7 @@
         <v>287</v>
       </c>
       <c r="C225" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>CB2.6-5</v>
       </c>
       <c r="D225" s="6"/>
@@ -13156,11 +13156,11 @@
         <v>6</v>
       </c>
       <c r="I225" s="5">
-        <f>SUMIF($C:$C,"="&amp;B225,J:J)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="J225" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="K225" s="5"/>
@@ -13192,7 +13192,7 @@
         <v>287</v>
       </c>
       <c r="C226" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>RS380-PH</v>
       </c>
       <c r="D226" s="6" t="s">
@@ -13211,11 +13211,11 @@
         <v>3</v>
       </c>
       <c r="I226" s="5">
-        <f>SUMIF($C:$C,"="&amp;B226,J:J)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="J226" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="K226" s="5" t="s">
@@ -13245,7 +13245,7 @@
         <v>287</v>
       </c>
       <c r="C227" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>SS0.5-10</v>
       </c>
       <c r="D227" s="6" t="s">
@@ -13264,11 +13264,11 @@
         <v>3</v>
       </c>
       <c r="I227" s="5">
-        <f>SUMIF($C:$C,"="&amp;B227,J:J)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="J227" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="K227" s="5"/>
@@ -13306,7 +13306,7 @@
         <v>287</v>
       </c>
       <c r="C228" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>CL-315BE</v>
       </c>
       <c r="D228" s="6" t="s">
@@ -13325,11 +13325,11 @@
         <v>4</v>
       </c>
       <c r="I228" s="5">
-        <f>SUMIF($C:$C,"="&amp;B228,J:J)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="J228" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="K228" s="5"/>
@@ -13367,7 +13367,7 @@
         <v>292</v>
       </c>
       <c r="C229" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>DP-C4x12</v>
       </c>
       <c r="D229" s="6" t="s">
@@ -13386,11 +13386,11 @@
         <v>8</v>
       </c>
       <c r="I229" s="5">
-        <f>SUMIF($C:$C,"="&amp;B229,J:J)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="J229" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="K229" s="5" t="s">
@@ -13420,7 +13420,7 @@
         <v>292</v>
       </c>
       <c r="C230" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>GEFHBB0.5-80-5-15-W0-LFC27-M6</v>
       </c>
       <c r="D230" s="6"/>
@@ -13437,11 +13437,11 @@
         <v>1</v>
       </c>
       <c r="I230" s="5">
-        <f>SUMIF($C:$C,"="&amp;B230,J:J)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="J230" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="K230" s="5"/>
@@ -13473,7 +13473,7 @@
         <v>292</v>
       </c>
       <c r="C231" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>BFLB4-5</v>
       </c>
       <c r="D231" s="6"/>
@@ -13490,11 +13490,11 @@
         <v>8</v>
       </c>
       <c r="I231" s="5">
-        <f>SUMIF($C:$C,"="&amp;B231,J:J)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="J231" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="K231" s="5"/>
@@ -13526,7 +13526,7 @@
         <v>292</v>
       </c>
       <c r="C232" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>B6809ZZ</v>
       </c>
       <c r="D232" s="6"/>
@@ -13543,11 +13543,11 @@
         <v>1</v>
       </c>
       <c r="I232" s="5">
-        <f>SUMIF($C:$C,"="&amp;B232,J:J)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="J232" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="K232" s="5"/>
@@ -13579,7 +13579,7 @@
         <v>292</v>
       </c>
       <c r="C233" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>B6700ZZ</v>
       </c>
       <c r="D233" s="6"/>
@@ -13596,11 +13596,11 @@
         <v>1</v>
       </c>
       <c r="I233" s="5">
-        <f>SUMIF($C:$C,"="&amp;B233,J:J)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="J233" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="K233" s="5"/>
@@ -13632,7 +13632,7 @@
         <v>292</v>
       </c>
       <c r="C234" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>B676ZZ</v>
       </c>
       <c r="D234" s="6"/>
@@ -13649,11 +13649,11 @@
         <v>1</v>
       </c>
       <c r="I234" s="5">
-        <f>SUMIF($C:$C,"="&amp;B234,J:J)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="J234" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="K234" s="5"/>
@@ -13685,7 +13685,7 @@
         <v>292</v>
       </c>
       <c r="C235" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>B6800ZZ</v>
       </c>
       <c r="D235" s="6"/>
@@ -13702,11 +13702,11 @@
         <v>1</v>
       </c>
       <c r="I235" s="5">
-        <f>SUMIF($C:$C,"="&amp;B235,J:J)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="J235" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="K235" s="5"/>
@@ -13738,7 +13738,7 @@
         <v>292</v>
       </c>
       <c r="C236" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>B6802ZZ</v>
       </c>
       <c r="D236" s="6"/>
@@ -13755,11 +13755,11 @@
         <v>1</v>
       </c>
       <c r="I236" s="5">
-        <f>SUMIF($C:$C,"="&amp;B236,J:J)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="J236" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="K236" s="5"/>
@@ -13791,7 +13791,7 @@
         <v>292</v>
       </c>
       <c r="C237" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>CBSTSR4-8</v>
       </c>
       <c r="D237" s="6"/>
@@ -13808,11 +13808,11 @@
         <v>1</v>
       </c>
       <c r="I237" s="5">
-        <f>SUMIF($C:$C,"="&amp;B237,J:J)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="J237" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="K237" s="5"/>
@@ -13844,7 +13844,7 @@
         <v>287</v>
       </c>
       <c r="C238" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>PWF3</v>
       </c>
       <c r="D238" s="6"/>
@@ -13859,11 +13859,11 @@
         <v>7</v>
       </c>
       <c r="I238" s="5">
-        <f>SUMIF($C:$C,"="&amp;B238,J:J)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="J238" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="K238" s="5"/>
@@ -13887,7 +13887,7 @@
         <v>287</v>
       </c>
       <c r="C239" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>SLW3</v>
       </c>
       <c r="D239" s="6"/>
@@ -13902,11 +13902,11 @@
         <v>7</v>
       </c>
       <c r="I239" s="5">
-        <f>SUMIF($C:$C,"="&amp;B239,J:J)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="J239" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="K239" s="5"/>
@@ -13944,11 +13944,11 @@
         <v>4</v>
       </c>
       <c r="I240" s="5">
-        <f>SUMIF($C:$C,"="&amp;B240,J:J)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="J240" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="K240" s="5"/>
@@ -13986,11 +13986,11 @@
         <v>3</v>
       </c>
       <c r="I241" s="5">
-        <f>SUMIF($C:$C,"="&amp;B241,J:J)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="J241" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="K241" s="5"/>
@@ -14022,7 +14022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C4C2C62-0CC6-46DF-A591-17DB98B93246}">
   <dimension ref="A1:C144"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -15904,7 +15904,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1F7574-C968-489E-91DC-0C793DF8D9FA}">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -16825,8 +16825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A131F5D-359C-447A-A38B-BF4A40019FE6}">
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25:H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -16988,6 +16988,7 @@
       <c r="G6" s="11" t="s">
         <v>343</v>
       </c>
+      <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7" t="str">
@@ -17156,6 +17157,7 @@
       <c r="G13" s="11" t="s">
         <v>356</v>
       </c>
+      <c r="H13" s="11"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" t="str">
@@ -17229,7 +17231,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A17" t="str">
         <v>CU-AAS-P003</v>
       </c>
@@ -17251,7 +17253,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A18" t="str">
         <v>CU-AAS-P004</v>
       </c>
@@ -17273,7 +17275,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A19" t="str">
         <v>CU-P001</v>
       </c>
@@ -17295,7 +17297,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A20" t="str">
         <v>CU-P002</v>
       </c>
@@ -17319,7 +17321,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A21" t="str">
         <v>CU-SAS001-P001</v>
       </c>
@@ -17344,8 +17346,9 @@
       <c r="G21" s="11" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H21" s="11"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A22" t="str">
         <v>CU-SAS001-P002</v>
       </c>
@@ -17369,7 +17372,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A23" t="str">
         <v>CU-SAS001-P003</v>
       </c>
@@ -17391,7 +17394,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A24" t="str">
         <v>CU-SAS002-P001</v>
       </c>
@@ -17417,7 +17420,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A25" t="str">
         <v>CU-SAS002-P002</v>
       </c>
@@ -17441,7 +17444,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A26" t="str">
         <v>CU-SAS002-P003</v>
       </c>
@@ -17465,7 +17468,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A27" t="str">
         <v>CU-SAS003-P001</v>
       </c>
@@ -17487,7 +17490,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A28" t="str">
         <v>CU-SAS003-P002</v>
       </c>
@@ -17509,7 +17512,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A29" t="str">
         <v>LS001-P001</v>
       </c>
@@ -17531,7 +17534,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A30" t="str">
         <v>LS-P002</v>
       </c>
@@ -17553,7 +17556,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A31" t="str">
         <v>LS-P003</v>
       </c>
@@ -17575,7 +17578,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A32" t="str">
         <v>LS-P004</v>
       </c>
@@ -17597,7 +17600,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A33" t="str">
         <v>LS-P005</v>
       </c>
@@ -17619,7 +17622,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A34" t="str">
         <v>R-HL-P001</v>
       </c>
@@ -17643,7 +17646,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A35" t="str">
         <v>R-HL-P002</v>
       </c>
@@ -17667,7 +17670,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A36" t="str">
         <v>R-HL-P003</v>
       </c>
@@ -17689,7 +17692,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A37" t="str">
         <v>R-HL-P004</v>
       </c>
@@ -17712,8 +17715,9 @@
       <c r="G37" s="11" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H37" s="11"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A38" t="str">
         <v>R-HL-P005</v>
       </c>
@@ -17735,7 +17739,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A39" t="str">
         <v>R-HL-P006</v>
       </c>
@@ -17760,8 +17764,9 @@
       <c r="G39" s="11" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H39" s="11"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A40" t="str">
         <v>R-HL-P007</v>
       </c>
@@ -17784,8 +17789,9 @@
       <c r="G40" s="11" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H40" s="11"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A41" t="str">
         <v>R-HL-RAS-P001</v>
       </c>
@@ -17808,8 +17814,9 @@
       <c r="G41" s="11" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H41" s="11"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A42" t="str">
         <v>R-HL-RAS-P002</v>
       </c>
@@ -17832,8 +17839,9 @@
       <c r="G42" s="11" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H42" s="11"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A43" t="str">
         <v>R-HL-RAS-P003</v>
       </c>
@@ -17855,7 +17863,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A44" t="str">
         <v>RL-P001</v>
       </c>
@@ -17880,8 +17888,9 @@
       <c r="G44" s="11" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H44" s="11"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A45" t="str">
         <v>RL-P002</v>
       </c>
@@ -17903,7 +17912,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A46" t="str">
         <v>R-P001</v>
       </c>
@@ -17928,8 +17937,9 @@
       <c r="G46" s="11" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H46" s="11"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A47" t="str">
         <v>R-P002</v>
       </c>
@@ -17950,8 +17960,9 @@
       <c r="G47" s="11" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H47" s="11"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A48" t="str">
         <v>R-P003</v>
       </c>
@@ -17973,7 +17984,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A49" t="str">
         <v>R-P004</v>
       </c>
@@ -17995,7 +18006,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A50" t="str">
         <v>R-P005</v>
       </c>
@@ -18017,7 +18028,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A51" t="str">
         <v>RR-HL-RAS-P001</v>
       </c>
@@ -18039,7 +18050,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A52" t="str">
         <v>RR-P001</v>
       </c>
@@ -18064,8 +18075,9 @@
       <c r="G52" s="11" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H52" s="11"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A53" t="str">
         <v>RR-P002</v>
       </c>
@@ -18087,7 +18099,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A54" t="str">
         <v>R-SA001-P001</v>
       </c>
@@ -18109,7 +18121,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A55" t="str">
         <v>R-SA001-P002</v>
       </c>
@@ -18131,7 +18143,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A56" t="str">
         <v>R-SA001-P003</v>
       </c>
@@ -18156,8 +18168,9 @@
       <c r="G56" s="11" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H56" s="11"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A57" t="str">
         <v>レシーバ v1</v>
       </c>
@@ -18176,7 +18189,7 @@
       <c r="E57" s="9"/>
       <c r="F57" s="9"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A58" t="str">
         <v>右足駆動回路v2</v>
       </c>
@@ -18195,7 +18208,7 @@
       <c r="E58" s="9"/>
       <c r="F58" s="9"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A59" t="str">
         <v>左足駆動回路v2</v>
       </c>

</xml_diff>